<commit_message>
Regenerated SML and ES outputs after merge
</commit_message>
<xml_diff>
--- a/output/EventSummary/encounter-es-1.xlsx
+++ b/output/EventSummary/encounter-es-1.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2686" uniqueCount="434">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2686" uniqueCount="433">
   <si>
     <t>Path</t>
   </si>
@@ -349,7 +349,7 @@
   </si>
   <si>
     <t>ele-1:All FHIR elements must have a @value or children {hasValue() | (children().count() &gt; id.count())}
-ext-1:Must have either extensions or value[x], not both {extension.exists() != value.exists()}ele-1:All FHIR elements must have a @value or children {hasValue() | (children().count() &gt; id.count())}ext-1:Must have either extensions or value[x], not both {extension.exists() != value.exists()}</t>
+ext-1:Must have either extensions or value[x], not both {extension.exists() != value.exists()}</t>
   </si>
   <si>
     <t>associatedHealthcareService</t>
@@ -363,10 +363,6 @@
   </si>
   <si>
     <t>Healthcare service relating to a resource.</t>
-  </si>
-  <si>
-    <t>ele-1:All FHIR elements must have a @value or children {hasValue() | (children().count() &gt; id.count())}
-ext-1:Must have either extensions or value[x], not both {extension.exists() != value.exists()}</t>
   </si>
   <si>
     <t>Encounter.modifierExtension</t>
@@ -2742,7 +2738,7 @@
         <v>104</v>
       </c>
       <c r="AI11" t="s" s="2">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="AJ11" t="s" s="2">
         <v>42</v>
@@ -2756,11 +2752,11 @@
     </row>
     <row r="12" hidden="true">
       <c r="A12" t="s" s="2">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" t="s" s="2">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D12" s="2"/>
       <c r="E12" t="s" s="2">
@@ -2782,13 +2778,13 @@
         <v>94</v>
       </c>
       <c r="K12" t="s" s="2">
+        <v>112</v>
+      </c>
+      <c r="L12" t="s" s="2">
         <v>113</v>
       </c>
-      <c r="L12" t="s" s="2">
+      <c r="M12" t="s" s="2">
         <v>114</v>
-      </c>
-      <c r="M12" t="s" s="2">
-        <v>115</v>
       </c>
       <c r="N12" s="2"/>
       <c r="O12" t="s" s="2">
@@ -2838,7 +2834,7 @@
         <v>42</v>
       </c>
       <c r="AE12" t="s" s="2">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="AF12" t="s" s="2">
         <v>40</v>
@@ -2864,7 +2860,7 @@
     </row>
     <row r="13" hidden="true">
       <c r="A13" t="s" s="2">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" t="s" s="2">
@@ -2887,13 +2883,13 @@
         <v>50</v>
       </c>
       <c r="J13" t="s" s="2">
+        <v>117</v>
+      </c>
+      <c r="K13" t="s" s="2">
         <v>118</v>
       </c>
-      <c r="K13" t="s" s="2">
+      <c r="L13" t="s" s="2">
         <v>119</v>
-      </c>
-      <c r="L13" t="s" s="2">
-        <v>120</v>
       </c>
       <c r="M13" s="2"/>
       <c r="N13" s="2"/>
@@ -2944,7 +2940,7 @@
         <v>42</v>
       </c>
       <c r="AE13" t="s" s="2">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="AF13" t="s" s="2">
         <v>40</v>
@@ -2959,18 +2955,18 @@
         <v>42</v>
       </c>
       <c r="AJ13" t="s" s="2">
+        <v>120</v>
+      </c>
+      <c r="AK13" t="s" s="2">
         <v>121</v>
       </c>
-      <c r="AK13" t="s" s="2">
+      <c r="AL13" t="s" s="2">
         <v>122</v>
-      </c>
-      <c r="AL13" t="s" s="2">
-        <v>123</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="2">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" t="s" s="2">
@@ -2996,13 +2992,13 @@
         <v>68</v>
       </c>
       <c r="K14" t="s" s="2">
+        <v>124</v>
+      </c>
+      <c r="L14" t="s" s="2">
         <v>125</v>
       </c>
-      <c r="L14" t="s" s="2">
+      <c r="M14" t="s" s="2">
         <v>126</v>
-      </c>
-      <c r="M14" t="s" s="2">
-        <v>127</v>
       </c>
       <c r="N14" s="2"/>
       <c r="O14" t="s" s="2">
@@ -3028,14 +3024,14 @@
         <v>42</v>
       </c>
       <c r="W14" t="s" s="2">
+        <v>127</v>
+      </c>
+      <c r="X14" t="s" s="2">
         <v>128</v>
       </c>
-      <c r="X14" t="s" s="2">
+      <c r="Y14" t="s" s="2">
         <v>129</v>
       </c>
-      <c r="Y14" t="s" s="2">
-        <v>130</v>
-      </c>
       <c r="Z14" t="s" s="2">
         <v>42</v>
       </c>
@@ -3052,7 +3048,7 @@
         <v>42</v>
       </c>
       <c r="AE14" t="s" s="2">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="AF14" t="s" s="2">
         <v>49</v>
@@ -3067,18 +3063,18 @@
         <v>42</v>
       </c>
       <c r="AJ14" t="s" s="2">
+        <v>130</v>
+      </c>
+      <c r="AK14" t="s" s="2">
         <v>131</v>
       </c>
-      <c r="AK14" t="s" s="2">
+      <c r="AL14" t="s" s="2">
         <v>132</v>
-      </c>
-      <c r="AL14" t="s" s="2">
-        <v>133</v>
       </c>
     </row>
     <row r="15" hidden="true">
       <c r="A15" t="s" s="2">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" t="s" s="2">
@@ -3101,16 +3097,16 @@
         <v>42</v>
       </c>
       <c r="J15" t="s" s="2">
+        <v>134</v>
+      </c>
+      <c r="K15" t="s" s="2">
         <v>135</v>
       </c>
-      <c r="K15" t="s" s="2">
+      <c r="L15" t="s" s="2">
         <v>136</v>
       </c>
-      <c r="L15" t="s" s="2">
+      <c r="M15" t="s" s="2">
         <v>137</v>
-      </c>
-      <c r="M15" t="s" s="2">
-        <v>138</v>
       </c>
       <c r="N15" s="2"/>
       <c r="O15" t="s" s="2">
@@ -3160,7 +3156,7 @@
         <v>42</v>
       </c>
       <c r="AE15" t="s" s="2">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="AF15" t="s" s="2">
         <v>40</v>
@@ -3172,10 +3168,10 @@
         <v>42</v>
       </c>
       <c r="AI15" t="s" s="2">
+        <v>138</v>
+      </c>
+      <c r="AJ15" t="s" s="2">
         <v>139</v>
-      </c>
-      <c r="AJ15" t="s" s="2">
-        <v>140</v>
       </c>
       <c r="AK15" t="s" s="2">
         <v>42</v>
@@ -3186,7 +3182,7 @@
     </row>
     <row r="16" hidden="true">
       <c r="A16" t="s" s="2">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" t="s" s="2">
@@ -3209,13 +3205,13 @@
         <v>42</v>
       </c>
       <c r="J16" t="s" s="2">
+        <v>141</v>
+      </c>
+      <c r="K16" t="s" s="2">
         <v>142</v>
       </c>
-      <c r="K16" t="s" s="2">
+      <c r="L16" t="s" s="2">
         <v>143</v>
-      </c>
-      <c r="L16" t="s" s="2">
-        <v>144</v>
       </c>
       <c r="M16" s="2"/>
       <c r="N16" s="2"/>
@@ -3266,7 +3262,7 @@
         <v>42</v>
       </c>
       <c r="AE16" t="s" s="2">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="AF16" t="s" s="2">
         <v>40</v>
@@ -3281,7 +3277,7 @@
         <v>42</v>
       </c>
       <c r="AJ16" t="s" s="2">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AK16" t="s" s="2">
         <v>42</v>
@@ -3292,11 +3288,11 @@
     </row>
     <row r="17" hidden="true">
       <c r="A17" t="s" s="2">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" t="s" s="2">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D17" s="2"/>
       <c r="E17" t="s" s="2">
@@ -3318,13 +3314,13 @@
         <v>94</v>
       </c>
       <c r="K17" t="s" s="2">
+        <v>146</v>
+      </c>
+      <c r="L17" t="s" s="2">
         <v>147</v>
       </c>
-      <c r="L17" t="s" s="2">
-        <v>148</v>
-      </c>
       <c r="M17" t="s" s="2">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="N17" s="2"/>
       <c r="O17" t="s" s="2">
@@ -3374,7 +3370,7 @@
         <v>42</v>
       </c>
       <c r="AE17" t="s" s="2">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="AF17" t="s" s="2">
         <v>40</v>
@@ -3389,7 +3385,7 @@
         <v>42</v>
       </c>
       <c r="AJ17" t="s" s="2">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AK17" t="s" s="2">
         <v>42</v>
@@ -3400,11 +3396,11 @@
     </row>
     <row r="18" hidden="true">
       <c r="A18" t="s" s="2">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" t="s" s="2">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D18" s="2"/>
       <c r="E18" t="s" s="2">
@@ -3426,13 +3422,13 @@
         <v>94</v>
       </c>
       <c r="K18" t="s" s="2">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="L18" t="s" s="2">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="M18" t="s" s="2">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="N18" s="2"/>
       <c r="O18" t="s" s="2">
@@ -3482,7 +3478,7 @@
         <v>42</v>
       </c>
       <c r="AE18" t="s" s="2">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AF18" t="s" s="2">
         <v>40</v>
@@ -3508,7 +3504,7 @@
     </row>
     <row r="19" hidden="true">
       <c r="A19" t="s" s="2">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" t="s" s="2">
@@ -3534,10 +3530,10 @@
         <v>68</v>
       </c>
       <c r="K19" t="s" s="2">
+        <v>124</v>
+      </c>
+      <c r="L19" t="s" s="2">
         <v>125</v>
-      </c>
-      <c r="L19" t="s" s="2">
-        <v>126</v>
       </c>
       <c r="M19" s="2"/>
       <c r="N19" s="2"/>
@@ -3564,14 +3560,14 @@
         <v>42</v>
       </c>
       <c r="W19" t="s" s="2">
+        <v>127</v>
+      </c>
+      <c r="X19" t="s" s="2">
         <v>128</v>
       </c>
-      <c r="X19" t="s" s="2">
+      <c r="Y19" t="s" s="2">
         <v>129</v>
       </c>
-      <c r="Y19" t="s" s="2">
-        <v>130</v>
-      </c>
       <c r="Z19" t="s" s="2">
         <v>42</v>
       </c>
@@ -3588,7 +3584,7 @@
         <v>42</v>
       </c>
       <c r="AE19" t="s" s="2">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AF19" t="s" s="2">
         <v>49</v>
@@ -3603,7 +3599,7 @@
         <v>42</v>
       </c>
       <c r="AJ19" t="s" s="2">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AK19" t="s" s="2">
         <v>42</v>
@@ -3614,7 +3610,7 @@
     </row>
     <row r="20" hidden="true">
       <c r="A20" t="s" s="2">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" t="s" s="2">
@@ -3637,13 +3633,13 @@
         <v>42</v>
       </c>
       <c r="J20" t="s" s="2">
+        <v>155</v>
+      </c>
+      <c r="K20" t="s" s="2">
         <v>156</v>
       </c>
-      <c r="K20" t="s" s="2">
+      <c r="L20" t="s" s="2">
         <v>157</v>
-      </c>
-      <c r="L20" t="s" s="2">
-        <v>158</v>
       </c>
       <c r="M20" s="2"/>
       <c r="N20" s="2"/>
@@ -3694,7 +3690,7 @@
         <v>42</v>
       </c>
       <c r="AE20" t="s" s="2">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="AF20" t="s" s="2">
         <v>49</v>
@@ -3709,7 +3705,7 @@
         <v>42</v>
       </c>
       <c r="AJ20" t="s" s="2">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AK20" t="s" s="2">
         <v>42</v>
@@ -3720,7 +3716,7 @@
     </row>
     <row r="21">
       <c r="A21" t="s" s="2">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" t="s" s="2">
@@ -3743,13 +3739,13 @@
         <v>50</v>
       </c>
       <c r="J21" t="s" s="2">
+        <v>159</v>
+      </c>
+      <c r="K21" t="s" s="2">
         <v>160</v>
       </c>
-      <c r="K21" t="s" s="2">
+      <c r="L21" t="s" s="2">
         <v>161</v>
-      </c>
-      <c r="L21" t="s" s="2">
-        <v>162</v>
       </c>
       <c r="M21" s="2"/>
       <c r="N21" s="2"/>
@@ -3779,11 +3775,11 @@
         <v>72</v>
       </c>
       <c r="X21" t="s" s="2">
+        <v>162</v>
+      </c>
+      <c r="Y21" t="s" s="2">
         <v>163</v>
       </c>
-      <c r="Y21" t="s" s="2">
-        <v>164</v>
-      </c>
       <c r="Z21" t="s" s="2">
         <v>42</v>
       </c>
@@ -3800,7 +3796,7 @@
         <v>42</v>
       </c>
       <c r="AE21" t="s" s="2">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="AF21" t="s" s="2">
         <v>40</v>
@@ -3815,18 +3811,18 @@
         <v>42</v>
       </c>
       <c r="AJ21" t="s" s="2">
+        <v>164</v>
+      </c>
+      <c r="AK21" t="s" s="2">
         <v>165</v>
       </c>
-      <c r="AK21" t="s" s="2">
+      <c r="AL21" t="s" s="2">
         <v>166</v>
-      </c>
-      <c r="AL21" t="s" s="2">
-        <v>167</v>
       </c>
     </row>
     <row r="22" hidden="true">
       <c r="A22" t="s" s="2">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" t="s" s="2">
@@ -3849,13 +3845,13 @@
         <v>42</v>
       </c>
       <c r="J22" t="s" s="2">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K22" t="s" s="2">
+        <v>168</v>
+      </c>
+      <c r="L22" t="s" s="2">
         <v>169</v>
-      </c>
-      <c r="L22" t="s" s="2">
-        <v>170</v>
       </c>
       <c r="M22" s="2"/>
       <c r="N22" s="2"/>
@@ -3906,7 +3902,7 @@
         <v>42</v>
       </c>
       <c r="AE22" t="s" s="2">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="AF22" t="s" s="2">
         <v>40</v>
@@ -3918,10 +3914,10 @@
         <v>42</v>
       </c>
       <c r="AI22" t="s" s="2">
+        <v>138</v>
+      </c>
+      <c r="AJ22" t="s" s="2">
         <v>139</v>
-      </c>
-      <c r="AJ22" t="s" s="2">
-        <v>140</v>
       </c>
       <c r="AK22" t="s" s="2">
         <v>42</v>
@@ -3932,7 +3928,7 @@
     </row>
     <row r="23" hidden="true">
       <c r="A23" t="s" s="2">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" t="s" s="2">
@@ -3955,13 +3951,13 @@
         <v>42</v>
       </c>
       <c r="J23" t="s" s="2">
+        <v>141</v>
+      </c>
+      <c r="K23" t="s" s="2">
         <v>142</v>
       </c>
-      <c r="K23" t="s" s="2">
+      <c r="L23" t="s" s="2">
         <v>143</v>
-      </c>
-      <c r="L23" t="s" s="2">
-        <v>144</v>
       </c>
       <c r="M23" s="2"/>
       <c r="N23" s="2"/>
@@ -4012,7 +4008,7 @@
         <v>42</v>
       </c>
       <c r="AE23" t="s" s="2">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="AF23" t="s" s="2">
         <v>40</v>
@@ -4027,7 +4023,7 @@
         <v>42</v>
       </c>
       <c r="AJ23" t="s" s="2">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AK23" t="s" s="2">
         <v>42</v>
@@ -4038,11 +4034,11 @@
     </row>
     <row r="24" hidden="true">
       <c r="A24" t="s" s="2">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" t="s" s="2">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D24" s="2"/>
       <c r="E24" t="s" s="2">
@@ -4064,13 +4060,13 @@
         <v>94</v>
       </c>
       <c r="K24" t="s" s="2">
+        <v>146</v>
+      </c>
+      <c r="L24" t="s" s="2">
         <v>147</v>
       </c>
-      <c r="L24" t="s" s="2">
-        <v>148</v>
-      </c>
       <c r="M24" t="s" s="2">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="N24" s="2"/>
       <c r="O24" t="s" s="2">
@@ -4120,7 +4116,7 @@
         <v>42</v>
       </c>
       <c r="AE24" t="s" s="2">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="AF24" t="s" s="2">
         <v>40</v>
@@ -4135,7 +4131,7 @@
         <v>42</v>
       </c>
       <c r="AJ24" t="s" s="2">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AK24" t="s" s="2">
         <v>42</v>
@@ -4146,11 +4142,11 @@
     </row>
     <row r="25" hidden="true">
       <c r="A25" t="s" s="2">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" t="s" s="2">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D25" s="2"/>
       <c r="E25" t="s" s="2">
@@ -4172,13 +4168,13 @@
         <v>94</v>
       </c>
       <c r="K25" t="s" s="2">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="L25" t="s" s="2">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="M25" t="s" s="2">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="N25" s="2"/>
       <c r="O25" t="s" s="2">
@@ -4228,7 +4224,7 @@
         <v>42</v>
       </c>
       <c r="AE25" t="s" s="2">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AF25" t="s" s="2">
         <v>40</v>
@@ -4254,7 +4250,7 @@
     </row>
     <row r="26" hidden="true">
       <c r="A26" t="s" s="2">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" t="s" s="2">
@@ -4277,13 +4273,13 @@
         <v>42</v>
       </c>
       <c r="J26" t="s" s="2">
+        <v>159</v>
+      </c>
+      <c r="K26" t="s" s="2">
         <v>160</v>
       </c>
-      <c r="K26" t="s" s="2">
+      <c r="L26" t="s" s="2">
         <v>161</v>
-      </c>
-      <c r="L26" t="s" s="2">
-        <v>162</v>
       </c>
       <c r="M26" s="2"/>
       <c r="N26" s="2"/>
@@ -4313,11 +4309,11 @@
         <v>72</v>
       </c>
       <c r="X26" t="s" s="2">
+        <v>162</v>
+      </c>
+      <c r="Y26" t="s" s="2">
         <v>163</v>
       </c>
-      <c r="Y26" t="s" s="2">
-        <v>164</v>
-      </c>
       <c r="Z26" t="s" s="2">
         <v>42</v>
       </c>
@@ -4334,7 +4330,7 @@
         <v>42</v>
       </c>
       <c r="AE26" t="s" s="2">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="AF26" t="s" s="2">
         <v>49</v>
@@ -4349,7 +4345,7 @@
         <v>42</v>
       </c>
       <c r="AJ26" t="s" s="2">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AK26" t="s" s="2">
         <v>42</v>
@@ -4360,7 +4356,7 @@
     </row>
     <row r="27" hidden="true">
       <c r="A27" t="s" s="2">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27" t="s" s="2">
@@ -4383,13 +4379,13 @@
         <v>42</v>
       </c>
       <c r="J27" t="s" s="2">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="K27" t="s" s="2">
+        <v>175</v>
+      </c>
+      <c r="L27" t="s" s="2">
         <v>176</v>
-      </c>
-      <c r="L27" t="s" s="2">
-        <v>177</v>
       </c>
       <c r="M27" s="2"/>
       <c r="N27" s="2"/>
@@ -4440,7 +4436,7 @@
         <v>42</v>
       </c>
       <c r="AE27" t="s" s="2">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="AF27" t="s" s="2">
         <v>49</v>
@@ -4455,7 +4451,7 @@
         <v>42</v>
       </c>
       <c r="AJ27" t="s" s="2">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AK27" t="s" s="2">
         <v>42</v>
@@ -4466,7 +4462,7 @@
     </row>
     <row r="28">
       <c r="A28" t="s" s="2">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" t="s" s="2">
@@ -4489,16 +4485,16 @@
         <v>50</v>
       </c>
       <c r="J28" t="s" s="2">
+        <v>178</v>
+      </c>
+      <c r="K28" t="s" s="2">
         <v>179</v>
       </c>
-      <c r="K28" t="s" s="2">
+      <c r="L28" t="s" s="2">
         <v>180</v>
       </c>
-      <c r="L28" t="s" s="2">
+      <c r="M28" t="s" s="2">
         <v>181</v>
-      </c>
-      <c r="M28" t="s" s="2">
-        <v>182</v>
       </c>
       <c r="N28" s="2"/>
       <c r="O28" t="s" s="2">
@@ -4524,14 +4520,14 @@
         <v>42</v>
       </c>
       <c r="W28" t="s" s="2">
+        <v>182</v>
+      </c>
+      <c r="X28" t="s" s="2">
         <v>183</v>
       </c>
-      <c r="X28" t="s" s="2">
+      <c r="Y28" t="s" s="2">
         <v>184</v>
       </c>
-      <c r="Y28" t="s" s="2">
-        <v>185</v>
-      </c>
       <c r="Z28" t="s" s="2">
         <v>42</v>
       </c>
@@ -4548,7 +4544,7 @@
         <v>42</v>
       </c>
       <c r="AE28" t="s" s="2">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="AF28" t="s" s="2">
         <v>40</v>
@@ -4563,18 +4559,18 @@
         <v>42</v>
       </c>
       <c r="AJ28" t="s" s="2">
+        <v>185</v>
+      </c>
+      <c r="AK28" t="s" s="2">
+        <v>165</v>
+      </c>
+      <c r="AL28" t="s" s="2">
         <v>186</v>
-      </c>
-      <c r="AK28" t="s" s="2">
-        <v>166</v>
-      </c>
-      <c r="AL28" t="s" s="2">
-        <v>187</v>
       </c>
     </row>
     <row r="29" hidden="true">
       <c r="A29" t="s" s="2">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" t="s" s="2">
@@ -4597,13 +4593,13 @@
         <v>42</v>
       </c>
       <c r="J29" t="s" s="2">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="K29" t="s" s="2">
+        <v>188</v>
+      </c>
+      <c r="L29" t="s" s="2">
         <v>189</v>
-      </c>
-      <c r="L29" t="s" s="2">
-        <v>190</v>
       </c>
       <c r="M29" s="2"/>
       <c r="N29" s="2"/>
@@ -4630,14 +4626,14 @@
         <v>42</v>
       </c>
       <c r="W29" t="s" s="2">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="X29" t="s" s="2">
+        <v>189</v>
+      </c>
+      <c r="Y29" t="s" s="2">
         <v>190</v>
       </c>
-      <c r="Y29" t="s" s="2">
-        <v>191</v>
-      </c>
       <c r="Z29" t="s" s="2">
         <v>42</v>
       </c>
@@ -4654,7 +4650,7 @@
         <v>42</v>
       </c>
       <c r="AE29" t="s" s="2">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="AF29" t="s" s="2">
         <v>40</v>
@@ -4669,22 +4665,22 @@
         <v>42</v>
       </c>
       <c r="AJ29" t="s" s="2">
+        <v>191</v>
+      </c>
+      <c r="AK29" t="s" s="2">
         <v>192</v>
       </c>
-      <c r="AK29" t="s" s="2">
+      <c r="AL29" t="s" s="2">
         <v>193</v>
-      </c>
-      <c r="AL29" t="s" s="2">
-        <v>194</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s" s="2">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B30" s="2"/>
       <c r="C30" t="s" s="2">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D30" s="2"/>
       <c r="E30" t="s" s="2">
@@ -4703,16 +4699,16 @@
         <v>50</v>
       </c>
       <c r="J30" t="s" s="2">
+        <v>196</v>
+      </c>
+      <c r="K30" t="s" s="2">
         <v>197</v>
       </c>
-      <c r="K30" t="s" s="2">
+      <c r="L30" t="s" s="2">
         <v>198</v>
       </c>
-      <c r="L30" t="s" s="2">
+      <c r="M30" t="s" s="2">
         <v>199</v>
-      </c>
-      <c r="M30" t="s" s="2">
-        <v>200</v>
       </c>
       <c r="N30" s="2"/>
       <c r="O30" t="s" s="2">
@@ -4762,7 +4758,7 @@
         <v>42</v>
       </c>
       <c r="AE30" t="s" s="2">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="AF30" t="s" s="2">
         <v>40</v>
@@ -4777,18 +4773,18 @@
         <v>42</v>
       </c>
       <c r="AJ30" t="s" s="2">
+        <v>200</v>
+      </c>
+      <c r="AK30" t="s" s="2">
         <v>201</v>
       </c>
-      <c r="AK30" t="s" s="2">
+      <c r="AL30" t="s" s="2">
         <v>202</v>
-      </c>
-      <c r="AL30" t="s" s="2">
-        <v>203</v>
       </c>
     </row>
     <row r="31" hidden="true">
       <c r="A31" t="s" s="2">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" t="s" s="2">
@@ -4811,13 +4807,13 @@
         <v>50</v>
       </c>
       <c r="J31" t="s" s="2">
+        <v>204</v>
+      </c>
+      <c r="K31" t="s" s="2">
         <v>205</v>
       </c>
-      <c r="K31" t="s" s="2">
+      <c r="L31" t="s" s="2">
         <v>206</v>
-      </c>
-      <c r="L31" t="s" s="2">
-        <v>207</v>
       </c>
       <c r="M31" s="2"/>
       <c r="N31" s="2"/>
@@ -4868,7 +4864,7 @@
         <v>42</v>
       </c>
       <c r="AE31" t="s" s="2">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="AF31" t="s" s="2">
         <v>40</v>
@@ -4883,18 +4879,18 @@
         <v>42</v>
       </c>
       <c r="AJ31" t="s" s="2">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AK31" t="s" s="2">
+        <v>207</v>
+      </c>
+      <c r="AL31" t="s" s="2">
         <v>208</v>
-      </c>
-      <c r="AL31" t="s" s="2">
-        <v>209</v>
       </c>
     </row>
     <row r="32" hidden="true">
       <c r="A32" t="s" s="2">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B32" s="2"/>
       <c r="C32" t="s" s="2">
@@ -4917,13 +4913,13 @@
         <v>42</v>
       </c>
       <c r="J32" t="s" s="2">
+        <v>210</v>
+      </c>
+      <c r="K32" t="s" s="2">
         <v>211</v>
       </c>
-      <c r="K32" t="s" s="2">
+      <c r="L32" t="s" s="2">
         <v>212</v>
-      </c>
-      <c r="L32" t="s" s="2">
-        <v>213</v>
       </c>
       <c r="M32" s="2"/>
       <c r="N32" s="2"/>
@@ -4974,7 +4970,7 @@
         <v>42</v>
       </c>
       <c r="AE32" t="s" s="2">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="AF32" t="s" s="2">
         <v>40</v>
@@ -4989,7 +4985,7 @@
         <v>42</v>
       </c>
       <c r="AJ32" t="s" s="2">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="AK32" t="s" s="2">
         <v>42</v>
@@ -5000,7 +4996,7 @@
     </row>
     <row r="33" hidden="true">
       <c r="A33" t="s" s="2">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" t="s" s="2">
@@ -5023,13 +5019,13 @@
         <v>50</v>
       </c>
       <c r="J33" t="s" s="2">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K33" t="s" s="2">
+        <v>215</v>
+      </c>
+      <c r="L33" t="s" s="2">
         <v>216</v>
-      </c>
-      <c r="L33" t="s" s="2">
-        <v>217</v>
       </c>
       <c r="M33" s="2"/>
       <c r="N33" s="2"/>
@@ -5080,7 +5076,7 @@
         <v>42</v>
       </c>
       <c r="AE33" t="s" s="2">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="AF33" t="s" s="2">
         <v>40</v>
@@ -5092,21 +5088,21 @@
         <v>42</v>
       </c>
       <c r="AI33" t="s" s="2">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="AJ33" t="s" s="2">
+        <v>217</v>
+      </c>
+      <c r="AK33" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AL33" t="s" s="2">
         <v>218</v>
-      </c>
-      <c r="AK33" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AL33" t="s" s="2">
-        <v>219</v>
       </c>
     </row>
     <row r="34" hidden="true">
       <c r="A34" t="s" s="2">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B34" s="2"/>
       <c r="C34" t="s" s="2">
@@ -5129,13 +5125,13 @@
         <v>42</v>
       </c>
       <c r="J34" t="s" s="2">
+        <v>141</v>
+      </c>
+      <c r="K34" t="s" s="2">
         <v>142</v>
       </c>
-      <c r="K34" t="s" s="2">
+      <c r="L34" t="s" s="2">
         <v>143</v>
-      </c>
-      <c r="L34" t="s" s="2">
-        <v>144</v>
       </c>
       <c r="M34" s="2"/>
       <c r="N34" s="2"/>
@@ -5186,7 +5182,7 @@
         <v>42</v>
       </c>
       <c r="AE34" t="s" s="2">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="AF34" t="s" s="2">
         <v>40</v>
@@ -5201,7 +5197,7 @@
         <v>42</v>
       </c>
       <c r="AJ34" t="s" s="2">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AK34" t="s" s="2">
         <v>42</v>
@@ -5212,11 +5208,11 @@
     </row>
     <row r="35" hidden="true">
       <c r="A35" t="s" s="2">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" t="s" s="2">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D35" s="2"/>
       <c r="E35" t="s" s="2">
@@ -5238,13 +5234,13 @@
         <v>94</v>
       </c>
       <c r="K35" t="s" s="2">
+        <v>146</v>
+      </c>
+      <c r="L35" t="s" s="2">
         <v>147</v>
       </c>
-      <c r="L35" t="s" s="2">
-        <v>148</v>
-      </c>
       <c r="M35" t="s" s="2">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="N35" s="2"/>
       <c r="O35" t="s" s="2">
@@ -5294,7 +5290,7 @@
         <v>42</v>
       </c>
       <c r="AE35" t="s" s="2">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="AF35" t="s" s="2">
         <v>40</v>
@@ -5309,7 +5305,7 @@
         <v>42</v>
       </c>
       <c r="AJ35" t="s" s="2">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AK35" t="s" s="2">
         <v>42</v>
@@ -5320,11 +5316,11 @@
     </row>
     <row r="36" hidden="true">
       <c r="A36" t="s" s="2">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B36" s="2"/>
       <c r="C36" t="s" s="2">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D36" s="2"/>
       <c r="E36" t="s" s="2">
@@ -5346,13 +5342,13 @@
         <v>94</v>
       </c>
       <c r="K36" t="s" s="2">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="L36" t="s" s="2">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="M36" t="s" s="2">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="N36" s="2"/>
       <c r="O36" t="s" s="2">
@@ -5402,7 +5398,7 @@
         <v>42</v>
       </c>
       <c r="AE36" t="s" s="2">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AF36" t="s" s="2">
         <v>40</v>
@@ -5428,7 +5424,7 @@
     </row>
     <row r="37" hidden="true">
       <c r="A37" t="s" s="2">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" t="s" s="2">
@@ -5451,16 +5447,16 @@
         <v>50</v>
       </c>
       <c r="J37" t="s" s="2">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="K37" t="s" s="2">
+        <v>223</v>
+      </c>
+      <c r="L37" t="s" s="2">
         <v>224</v>
       </c>
-      <c r="L37" t="s" s="2">
+      <c r="M37" t="s" s="2">
         <v>225</v>
-      </c>
-      <c r="M37" t="s" s="2">
-        <v>226</v>
       </c>
       <c r="N37" s="2"/>
       <c r="O37" t="s" s="2">
@@ -5489,10 +5485,10 @@
         <v>72</v>
       </c>
       <c r="X37" t="s" s="2">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="Y37" t="s" s="2">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="Z37" t="s" s="2">
         <v>42</v>
@@ -5510,7 +5506,7 @@
         <v>42</v>
       </c>
       <c r="AE37" t="s" s="2">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="AF37" t="s" s="2">
         <v>40</v>
@@ -5525,18 +5521,18 @@
         <v>42</v>
       </c>
       <c r="AJ37" t="s" s="2">
+        <v>227</v>
+      </c>
+      <c r="AK37" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AL37" t="s" s="2">
         <v>228</v>
-      </c>
-      <c r="AK37" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AL37" t="s" s="2">
-        <v>229</v>
       </c>
     </row>
     <row r="38" hidden="true">
       <c r="A38" t="s" s="2">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B38" s="2"/>
       <c r="C38" t="s" s="2">
@@ -5559,13 +5555,13 @@
         <v>42</v>
       </c>
       <c r="J38" t="s" s="2">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="K38" t="s" s="2">
+        <v>230</v>
+      </c>
+      <c r="L38" t="s" s="2">
         <v>231</v>
-      </c>
-      <c r="L38" t="s" s="2">
-        <v>232</v>
       </c>
       <c r="M38" s="2"/>
       <c r="N38" s="2"/>
@@ -5616,7 +5612,7 @@
         <v>42</v>
       </c>
       <c r="AE38" t="s" s="2">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="AF38" t="s" s="2">
         <v>40</v>
@@ -5631,18 +5627,18 @@
         <v>42</v>
       </c>
       <c r="AJ38" t="s" s="2">
+        <v>232</v>
+      </c>
+      <c r="AK38" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AL38" t="s" s="2">
         <v>233</v>
-      </c>
-      <c r="AK38" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AL38" t="s" s="2">
-        <v>234</v>
       </c>
     </row>
     <row r="39" hidden="true">
       <c r="A39" t="s" s="2">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B39" s="2"/>
       <c r="C39" t="s" s="2">
@@ -5665,13 +5661,13 @@
         <v>50</v>
       </c>
       <c r="J39" t="s" s="2">
+        <v>235</v>
+      </c>
+      <c r="K39" t="s" s="2">
         <v>236</v>
       </c>
-      <c r="K39" t="s" s="2">
+      <c r="L39" t="s" s="2">
         <v>237</v>
-      </c>
-      <c r="L39" t="s" s="2">
-        <v>238</v>
       </c>
       <c r="M39" s="2"/>
       <c r="N39" s="2"/>
@@ -5722,7 +5718,7 @@
         <v>42</v>
       </c>
       <c r="AE39" t="s" s="2">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="AF39" t="s" s="2">
         <v>40</v>
@@ -5737,18 +5733,18 @@
         <v>42</v>
       </c>
       <c r="AJ39" t="s" s="2">
+        <v>238</v>
+      </c>
+      <c r="AK39" t="s" s="2">
         <v>239</v>
       </c>
-      <c r="AK39" t="s" s="2">
+      <c r="AL39" t="s" s="2">
         <v>240</v>
-      </c>
-      <c r="AL39" t="s" s="2">
-        <v>241</v>
       </c>
     </row>
     <row r="40" hidden="true">
       <c r="A40" t="s" s="2">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B40" s="2"/>
       <c r="C40" t="s" s="2">
@@ -5771,13 +5767,13 @@
         <v>50</v>
       </c>
       <c r="J40" t="s" s="2">
+        <v>242</v>
+      </c>
+      <c r="K40" t="s" s="2">
         <v>243</v>
       </c>
-      <c r="K40" t="s" s="2">
+      <c r="L40" t="s" s="2">
         <v>244</v>
-      </c>
-      <c r="L40" t="s" s="2">
-        <v>245</v>
       </c>
       <c r="M40" s="2"/>
       <c r="N40" s="2"/>
@@ -5828,7 +5824,7 @@
         <v>42</v>
       </c>
       <c r="AE40" t="s" s="2">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="AF40" t="s" s="2">
         <v>40</v>
@@ -5843,18 +5839,18 @@
         <v>42</v>
       </c>
       <c r="AJ40" t="s" s="2">
+        <v>245</v>
+      </c>
+      <c r="AK40" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AL40" t="s" s="2">
         <v>246</v>
-      </c>
-      <c r="AK40" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AL40" t="s" s="2">
-        <v>247</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s" s="2">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" t="s" s="2">
@@ -5877,16 +5873,16 @@
         <v>42</v>
       </c>
       <c r="J41" t="s" s="2">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="K41" t="s" s="2">
+        <v>248</v>
+      </c>
+      <c r="L41" t="s" s="2">
         <v>249</v>
       </c>
-      <c r="L41" t="s" s="2">
+      <c r="M41" t="s" s="2">
         <v>250</v>
-      </c>
-      <c r="M41" t="s" s="2">
-        <v>251</v>
       </c>
       <c r="N41" s="2"/>
       <c r="O41" t="s" s="2">
@@ -5936,7 +5932,7 @@
         <v>42</v>
       </c>
       <c r="AE41" t="s" s="2">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="AF41" t="s" s="2">
         <v>40</v>
@@ -5951,18 +5947,18 @@
         <v>42</v>
       </c>
       <c r="AJ41" t="s" s="2">
+        <v>251</v>
+      </c>
+      <c r="AK41" t="s" s="2">
         <v>252</v>
       </c>
-      <c r="AK41" t="s" s="2">
+      <c r="AL41" t="s" s="2">
         <v>253</v>
-      </c>
-      <c r="AL41" t="s" s="2">
-        <v>254</v>
       </c>
     </row>
     <row r="42" hidden="true">
       <c r="A42" t="s" s="2">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B42" s="2"/>
       <c r="C42" t="s" s="2">
@@ -5985,16 +5981,16 @@
         <v>42</v>
       </c>
       <c r="J42" t="s" s="2">
+        <v>255</v>
+      </c>
+      <c r="K42" t="s" s="2">
         <v>256</v>
       </c>
-      <c r="K42" t="s" s="2">
+      <c r="L42" t="s" s="2">
         <v>257</v>
       </c>
-      <c r="L42" t="s" s="2">
+      <c r="M42" t="s" s="2">
         <v>258</v>
-      </c>
-      <c r="M42" t="s" s="2">
-        <v>259</v>
       </c>
       <c r="N42" s="2"/>
       <c r="O42" t="s" s="2">
@@ -6044,7 +6040,7 @@
         <v>42</v>
       </c>
       <c r="AE42" t="s" s="2">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="AF42" t="s" s="2">
         <v>40</v>
@@ -6059,22 +6055,22 @@
         <v>42</v>
       </c>
       <c r="AJ42" t="s" s="2">
+        <v>259</v>
+      </c>
+      <c r="AK42" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AL42" t="s" s="2">
         <v>260</v>
-      </c>
-      <c r="AK42" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AL42" t="s" s="2">
-        <v>261</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s" s="2">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" t="s" s="2">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D43" s="2"/>
       <c r="E43" t="s" s="2">
@@ -6093,16 +6089,16 @@
         <v>50</v>
       </c>
       <c r="J43" t="s" s="2">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="K43" t="s" s="2">
+        <v>263</v>
+      </c>
+      <c r="L43" t="s" s="2">
         <v>264</v>
       </c>
-      <c r="L43" t="s" s="2">
+      <c r="M43" t="s" s="2">
         <v>265</v>
-      </c>
-      <c r="M43" t="s" s="2">
-        <v>266</v>
       </c>
       <c r="N43" s="2"/>
       <c r="O43" t="s" s="2">
@@ -6128,14 +6124,14 @@
         <v>42</v>
       </c>
       <c r="W43" t="s" s="2">
+        <v>266</v>
+      </c>
+      <c r="X43" t="s" s="2">
         <v>267</v>
       </c>
-      <c r="X43" t="s" s="2">
+      <c r="Y43" t="s" s="2">
         <v>268</v>
       </c>
-      <c r="Y43" t="s" s="2">
-        <v>269</v>
-      </c>
       <c r="Z43" t="s" s="2">
         <v>42</v>
       </c>
@@ -6152,7 +6148,7 @@
         <v>42</v>
       </c>
       <c r="AE43" t="s" s="2">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="AF43" t="s" s="2">
         <v>40</v>
@@ -6167,18 +6163,18 @@
         <v>42</v>
       </c>
       <c r="AJ43" t="s" s="2">
+        <v>269</v>
+      </c>
+      <c r="AK43" t="s" s="2">
         <v>270</v>
       </c>
-      <c r="AK43" t="s" s="2">
+      <c r="AL43" t="s" s="2">
         <v>271</v>
-      </c>
-      <c r="AL43" t="s" s="2">
-        <v>272</v>
       </c>
     </row>
     <row r="44" hidden="true">
       <c r="A44" t="s" s="2">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B44" s="2"/>
       <c r="C44" t="s" s="2">
@@ -6201,13 +6197,13 @@
         <v>50</v>
       </c>
       <c r="J44" t="s" s="2">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K44" t="s" s="2">
+        <v>273</v>
+      </c>
+      <c r="L44" t="s" s="2">
         <v>274</v>
-      </c>
-      <c r="L44" t="s" s="2">
-        <v>275</v>
       </c>
       <c r="M44" s="2"/>
       <c r="N44" s="2"/>
@@ -6258,7 +6254,7 @@
         <v>42</v>
       </c>
       <c r="AE44" t="s" s="2">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="AF44" t="s" s="2">
         <v>40</v>
@@ -6270,10 +6266,10 @@
         <v>42</v>
       </c>
       <c r="AI44" t="s" s="2">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="AJ44" t="s" s="2">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="AK44" t="s" s="2">
         <v>42</v>
@@ -6284,7 +6280,7 @@
     </row>
     <row r="45" hidden="true">
       <c r="A45" t="s" s="2">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B45" s="2"/>
       <c r="C45" t="s" s="2">
@@ -6307,13 +6303,13 @@
         <v>42</v>
       </c>
       <c r="J45" t="s" s="2">
+        <v>141</v>
+      </c>
+      <c r="K45" t="s" s="2">
         <v>142</v>
       </c>
-      <c r="K45" t="s" s="2">
+      <c r="L45" t="s" s="2">
         <v>143</v>
-      </c>
-      <c r="L45" t="s" s="2">
-        <v>144</v>
       </c>
       <c r="M45" s="2"/>
       <c r="N45" s="2"/>
@@ -6364,7 +6360,7 @@
         <v>42</v>
       </c>
       <c r="AE45" t="s" s="2">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="AF45" t="s" s="2">
         <v>40</v>
@@ -6379,7 +6375,7 @@
         <v>42</v>
       </c>
       <c r="AJ45" t="s" s="2">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AK45" t="s" s="2">
         <v>42</v>
@@ -6390,11 +6386,11 @@
     </row>
     <row r="46" hidden="true">
       <c r="A46" t="s" s="2">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B46" s="2"/>
       <c r="C46" t="s" s="2">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D46" s="2"/>
       <c r="E46" t="s" s="2">
@@ -6416,13 +6412,13 @@
         <v>94</v>
       </c>
       <c r="K46" t="s" s="2">
+        <v>146</v>
+      </c>
+      <c r="L46" t="s" s="2">
         <v>147</v>
       </c>
-      <c r="L46" t="s" s="2">
-        <v>148</v>
-      </c>
       <c r="M46" t="s" s="2">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="N46" s="2"/>
       <c r="O46" t="s" s="2">
@@ -6472,7 +6468,7 @@
         <v>42</v>
       </c>
       <c r="AE46" t="s" s="2">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="AF46" t="s" s="2">
         <v>40</v>
@@ -6487,7 +6483,7 @@
         <v>42</v>
       </c>
       <c r="AJ46" t="s" s="2">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AK46" t="s" s="2">
         <v>42</v>
@@ -6498,11 +6494,11 @@
     </row>
     <row r="47" hidden="true">
       <c r="A47" t="s" s="2">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B47" s="2"/>
       <c r="C47" t="s" s="2">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D47" s="2"/>
       <c r="E47" t="s" s="2">
@@ -6524,13 +6520,13 @@
         <v>94</v>
       </c>
       <c r="K47" t="s" s="2">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="L47" t="s" s="2">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="M47" t="s" s="2">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="N47" s="2"/>
       <c r="O47" t="s" s="2">
@@ -6580,7 +6576,7 @@
         <v>42</v>
       </c>
       <c r="AE47" t="s" s="2">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AF47" t="s" s="2">
         <v>40</v>
@@ -6606,11 +6602,11 @@
     </row>
     <row r="48" hidden="true">
       <c r="A48" t="s" s="2">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B48" s="2"/>
       <c r="C48" t="s" s="2">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D48" s="2"/>
       <c r="E48" t="s" s="2">
@@ -6629,16 +6625,16 @@
         <v>42</v>
       </c>
       <c r="J48" t="s" s="2">
+        <v>281</v>
+      </c>
+      <c r="K48" t="s" s="2">
         <v>282</v>
       </c>
-      <c r="K48" t="s" s="2">
+      <c r="L48" t="s" s="2">
         <v>283</v>
       </c>
-      <c r="L48" t="s" s="2">
-        <v>284</v>
-      </c>
       <c r="M48" t="s" s="2">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="N48" s="2"/>
       <c r="O48" t="s" s="2">
@@ -6688,7 +6684,7 @@
         <v>42</v>
       </c>
       <c r="AE48" t="s" s="2">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="AF48" t="s" s="2">
         <v>49</v>
@@ -6703,18 +6699,18 @@
         <v>42</v>
       </c>
       <c r="AJ48" t="s" s="2">
+        <v>284</v>
+      </c>
+      <c r="AK48" t="s" s="2">
+        <v>270</v>
+      </c>
+      <c r="AL48" t="s" s="2">
         <v>285</v>
-      </c>
-      <c r="AK48" t="s" s="2">
-        <v>271</v>
-      </c>
-      <c r="AL48" t="s" s="2">
-        <v>286</v>
       </c>
     </row>
     <row r="49" hidden="true">
       <c r="A49" t="s" s="2">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B49" s="2"/>
       <c r="C49" t="s" s="2">
@@ -6737,13 +6733,13 @@
         <v>42</v>
       </c>
       <c r="J49" t="s" s="2">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="K49" t="s" s="2">
+        <v>287</v>
+      </c>
+      <c r="L49" t="s" s="2">
         <v>288</v>
-      </c>
-      <c r="L49" t="s" s="2">
-        <v>289</v>
       </c>
       <c r="M49" s="2"/>
       <c r="N49" s="2"/>
@@ -6770,14 +6766,14 @@
         <v>42</v>
       </c>
       <c r="W49" t="s" s="2">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="X49" t="s" s="2">
+        <v>289</v>
+      </c>
+      <c r="Y49" t="s" s="2">
         <v>290</v>
       </c>
-      <c r="Y49" t="s" s="2">
-        <v>291</v>
-      </c>
       <c r="Z49" t="s" s="2">
         <v>42</v>
       </c>
@@ -6794,7 +6790,7 @@
         <v>42</v>
       </c>
       <c r="AE49" t="s" s="2">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="AF49" t="s" s="2">
         <v>40</v>
@@ -6809,7 +6805,7 @@
         <v>42</v>
       </c>
       <c r="AJ49" t="s" s="2">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AK49" t="s" s="2">
         <v>42</v>
@@ -6820,7 +6816,7 @@
     </row>
     <row r="50" hidden="true">
       <c r="A50" t="s" s="2">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B50" s="2"/>
       <c r="C50" t="s" s="2">
@@ -6843,13 +6839,13 @@
         <v>42</v>
       </c>
       <c r="J50" t="s" s="2">
+        <v>292</v>
+      </c>
+      <c r="K50" t="s" s="2">
         <v>293</v>
       </c>
-      <c r="K50" t="s" s="2">
+      <c r="L50" t="s" s="2">
         <v>294</v>
-      </c>
-      <c r="L50" t="s" s="2">
-        <v>295</v>
       </c>
       <c r="M50" s="2"/>
       <c r="N50" s="2"/>
@@ -6900,7 +6896,7 @@
         <v>42</v>
       </c>
       <c r="AE50" t="s" s="2">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="AF50" t="s" s="2">
         <v>40</v>
@@ -6915,7 +6911,7 @@
         <v>42</v>
       </c>
       <c r="AJ50" t="s" s="2">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="AK50" t="s" s="2">
         <v>42</v>
@@ -6926,7 +6922,7 @@
     </row>
     <row r="51" hidden="true">
       <c r="A51" t="s" s="2">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B51" s="2"/>
       <c r="C51" t="s" s="2">
@@ -6949,16 +6945,16 @@
         <v>42</v>
       </c>
       <c r="J51" t="s" s="2">
+        <v>297</v>
+      </c>
+      <c r="K51" t="s" s="2">
         <v>298</v>
       </c>
-      <c r="K51" t="s" s="2">
+      <c r="L51" t="s" s="2">
         <v>299</v>
       </c>
-      <c r="L51" t="s" s="2">
+      <c r="M51" t="s" s="2">
         <v>300</v>
-      </c>
-      <c r="M51" t="s" s="2">
-        <v>301</v>
       </c>
       <c r="N51" s="2"/>
       <c r="O51" t="s" s="2">
@@ -7008,7 +7004,7 @@
         <v>42</v>
       </c>
       <c r="AE51" t="s" s="2">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="AF51" t="s" s="2">
         <v>40</v>
@@ -7023,7 +7019,7 @@
         <v>42</v>
       </c>
       <c r="AJ51" t="s" s="2">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="AK51" t="s" s="2">
         <v>42</v>
@@ -7034,7 +7030,7 @@
     </row>
     <row r="52" hidden="true">
       <c r="A52" t="s" s="2">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B52" s="2"/>
       <c r="C52" t="s" s="2">
@@ -7057,16 +7053,16 @@
         <v>42</v>
       </c>
       <c r="J52" t="s" s="2">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K52" t="s" s="2">
+        <v>303</v>
+      </c>
+      <c r="L52" t="s" s="2">
         <v>304</v>
       </c>
-      <c r="L52" t="s" s="2">
+      <c r="M52" t="s" s="2">
         <v>305</v>
-      </c>
-      <c r="M52" t="s" s="2">
-        <v>306</v>
       </c>
       <c r="N52" s="2"/>
       <c r="O52" t="s" s="2">
@@ -7116,7 +7112,7 @@
         <v>42</v>
       </c>
       <c r="AE52" t="s" s="2">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="AF52" t="s" s="2">
         <v>40</v>
@@ -7128,10 +7124,10 @@
         <v>42</v>
       </c>
       <c r="AI52" t="s" s="2">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="AJ52" t="s" s="2">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="AK52" t="s" s="2">
         <v>42</v>
@@ -7142,7 +7138,7 @@
     </row>
     <row r="53" hidden="true">
       <c r="A53" t="s" s="2">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B53" s="2"/>
       <c r="C53" t="s" s="2">
@@ -7165,13 +7161,13 @@
         <v>42</v>
       </c>
       <c r="J53" t="s" s="2">
+        <v>141</v>
+      </c>
+      <c r="K53" t="s" s="2">
         <v>142</v>
       </c>
-      <c r="K53" t="s" s="2">
+      <c r="L53" t="s" s="2">
         <v>143</v>
-      </c>
-      <c r="L53" t="s" s="2">
-        <v>144</v>
       </c>
       <c r="M53" s="2"/>
       <c r="N53" s="2"/>
@@ -7222,7 +7218,7 @@
         <v>42</v>
       </c>
       <c r="AE53" t="s" s="2">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="AF53" t="s" s="2">
         <v>40</v>
@@ -7237,7 +7233,7 @@
         <v>42</v>
       </c>
       <c r="AJ53" t="s" s="2">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AK53" t="s" s="2">
         <v>42</v>
@@ -7248,7 +7244,7 @@
     </row>
     <row r="54" hidden="true">
       <c r="A54" t="s" s="2">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B54" s="2"/>
       <c r="C54" t="s" s="2">
@@ -7326,7 +7322,7 @@
         <v>98</v>
       </c>
       <c r="AE54" t="s" s="2">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="AF54" t="s" s="2">
         <v>40</v>
@@ -7352,10 +7348,10 @@
     </row>
     <row r="55" hidden="true">
       <c r="A55" t="s" s="2">
+        <v>308</v>
+      </c>
+      <c r="B55" t="s" s="2">
         <v>309</v>
-      </c>
-      <c r="B55" t="s" s="2">
-        <v>310</v>
       </c>
       <c r="C55" t="s" s="2">
         <v>42</v>
@@ -7377,13 +7373,13 @@
         <v>42</v>
       </c>
       <c r="J55" t="s" s="2">
+        <v>310</v>
+      </c>
+      <c r="K55" t="s" s="2">
         <v>311</v>
       </c>
-      <c r="K55" t="s" s="2">
+      <c r="L55" t="s" s="2">
         <v>312</v>
-      </c>
-      <c r="L55" t="s" s="2">
-        <v>313</v>
       </c>
       <c r="M55" s="2"/>
       <c r="N55" s="2"/>
@@ -7434,7 +7430,7 @@
         <v>42</v>
       </c>
       <c r="AE55" t="s" s="2">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="AF55" t="s" s="2">
         <v>40</v>
@@ -7446,7 +7442,7 @@
         <v>104</v>
       </c>
       <c r="AI55" t="s" s="2">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="AJ55" t="s" s="2">
         <v>42</v>
@@ -7460,10 +7456,10 @@
     </row>
     <row r="56" hidden="true">
       <c r="A56" t="s" s="2">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B56" t="s" s="2">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C56" t="s" s="2">
         <v>42</v>
@@ -7485,13 +7481,13 @@
         <v>42</v>
       </c>
       <c r="J56" t="s" s="2">
+        <v>314</v>
+      </c>
+      <c r="K56" t="s" s="2">
         <v>315</v>
       </c>
-      <c r="K56" t="s" s="2">
+      <c r="L56" t="s" s="2">
         <v>316</v>
-      </c>
-      <c r="L56" t="s" s="2">
-        <v>317</v>
       </c>
       <c r="M56" s="2"/>
       <c r="N56" s="2"/>
@@ -7542,7 +7538,7 @@
         <v>42</v>
       </c>
       <c r="AE56" t="s" s="2">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="AF56" t="s" s="2">
         <v>40</v>
@@ -7554,7 +7550,7 @@
         <v>104</v>
       </c>
       <c r="AI56" t="s" s="2">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="AJ56" t="s" s="2">
         <v>42</v>
@@ -7568,11 +7564,11 @@
     </row>
     <row r="57" hidden="true">
       <c r="A57" t="s" s="2">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B57" s="2"/>
       <c r="C57" t="s" s="2">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D57" s="2"/>
       <c r="E57" t="s" s="2">
@@ -7594,13 +7590,13 @@
         <v>94</v>
       </c>
       <c r="K57" t="s" s="2">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="L57" t="s" s="2">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="M57" t="s" s="2">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="N57" s="2"/>
       <c r="O57" t="s" s="2">
@@ -7650,7 +7646,7 @@
         <v>42</v>
       </c>
       <c r="AE57" t="s" s="2">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AF57" t="s" s="2">
         <v>40</v>
@@ -7676,7 +7672,7 @@
     </row>
     <row r="58" hidden="true">
       <c r="A58" t="s" s="2">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B58" s="2"/>
       <c r="C58" t="s" s="2">
@@ -7699,13 +7695,13 @@
         <v>42</v>
       </c>
       <c r="J58" t="s" s="2">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="K58" t="s" s="2">
+        <v>319</v>
+      </c>
+      <c r="L58" t="s" s="2">
         <v>320</v>
-      </c>
-      <c r="L58" t="s" s="2">
-        <v>321</v>
       </c>
       <c r="M58" s="2"/>
       <c r="N58" s="2"/>
@@ -7756,7 +7752,7 @@
         <v>42</v>
       </c>
       <c r="AE58" t="s" s="2">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="AF58" t="s" s="2">
         <v>40</v>
@@ -7771,18 +7767,18 @@
         <v>42</v>
       </c>
       <c r="AJ58" t="s" s="2">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="AK58" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AL58" t="s" s="2">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="59" hidden="true">
       <c r="A59" t="s" s="2">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B59" s="2"/>
       <c r="C59" t="s" s="2">
@@ -7805,13 +7801,13 @@
         <v>42</v>
       </c>
       <c r="J59" t="s" s="2">
+        <v>323</v>
+      </c>
+      <c r="K59" t="s" s="2">
         <v>324</v>
       </c>
-      <c r="K59" t="s" s="2">
+      <c r="L59" t="s" s="2">
         <v>325</v>
-      </c>
-      <c r="L59" t="s" s="2">
-        <v>326</v>
       </c>
       <c r="M59" s="2"/>
       <c r="N59" s="2"/>
@@ -7862,7 +7858,7 @@
         <v>42</v>
       </c>
       <c r="AE59" t="s" s="2">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="AF59" t="s" s="2">
         <v>40</v>
@@ -7877,7 +7873,7 @@
         <v>42</v>
       </c>
       <c r="AJ59" t="s" s="2">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="AK59" t="s" s="2">
         <v>42</v>
@@ -7888,7 +7884,7 @@
     </row>
     <row r="60" hidden="true">
       <c r="A60" t="s" s="2">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B60" s="2"/>
       <c r="C60" t="s" s="2">
@@ -7911,13 +7907,13 @@
         <v>42</v>
       </c>
       <c r="J60" t="s" s="2">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="K60" t="s" s="2">
+        <v>328</v>
+      </c>
+      <c r="L60" t="s" s="2">
         <v>329</v>
-      </c>
-      <c r="L60" t="s" s="2">
-        <v>330</v>
       </c>
       <c r="M60" s="2"/>
       <c r="N60" s="2"/>
@@ -7944,14 +7940,14 @@
         <v>42</v>
       </c>
       <c r="W60" t="s" s="2">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="X60" t="s" s="2">
+        <v>330</v>
+      </c>
+      <c r="Y60" t="s" s="2">
         <v>331</v>
       </c>
-      <c r="Y60" t="s" s="2">
-        <v>332</v>
-      </c>
       <c r="Z60" t="s" s="2">
         <v>42</v>
       </c>
@@ -7968,7 +7964,7 @@
         <v>42</v>
       </c>
       <c r="AE60" t="s" s="2">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="AF60" t="s" s="2">
         <v>40</v>
@@ -7983,18 +7979,18 @@
         <v>42</v>
       </c>
       <c r="AJ60" t="s" s="2">
+        <v>332</v>
+      </c>
+      <c r="AK60" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AL60" t="s" s="2">
         <v>333</v>
-      </c>
-      <c r="AK60" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AL60" t="s" s="2">
-        <v>334</v>
       </c>
     </row>
     <row r="61" hidden="true">
       <c r="A61" t="s" s="2">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B61" s="2"/>
       <c r="C61" t="s" s="2">
@@ -8017,13 +8013,13 @@
         <v>42</v>
       </c>
       <c r="J61" t="s" s="2">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="K61" t="s" s="2">
+        <v>335</v>
+      </c>
+      <c r="L61" t="s" s="2">
         <v>336</v>
-      </c>
-      <c r="L61" t="s" s="2">
-        <v>337</v>
       </c>
       <c r="M61" s="2"/>
       <c r="N61" s="2"/>
@@ -8050,14 +8046,14 @@
         <v>42</v>
       </c>
       <c r="W61" t="s" s="2">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="X61" t="s" s="2">
+        <v>337</v>
+      </c>
+      <c r="Y61" t="s" s="2">
         <v>338</v>
       </c>
-      <c r="Y61" t="s" s="2">
-        <v>339</v>
-      </c>
       <c r="Z61" t="s" s="2">
         <v>42</v>
       </c>
@@ -8074,7 +8070,7 @@
         <v>42</v>
       </c>
       <c r="AE61" t="s" s="2">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="AF61" t="s" s="2">
         <v>40</v>
@@ -8089,18 +8085,18 @@
         <v>42</v>
       </c>
       <c r="AJ61" t="s" s="2">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AK61" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AL61" t="s" s="2">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="62" hidden="true">
       <c r="A62" t="s" s="2">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B62" s="2"/>
       <c r="C62" t="s" s="2">
@@ -8123,19 +8119,19 @@
         <v>42</v>
       </c>
       <c r="J62" t="s" s="2">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="K62" t="s" s="2">
+        <v>341</v>
+      </c>
+      <c r="L62" t="s" s="2">
         <v>342</v>
       </c>
-      <c r="L62" t="s" s="2">
+      <c r="M62" t="s" s="2">
         <v>343</v>
       </c>
-      <c r="M62" t="s" s="2">
+      <c r="N62" t="s" s="2">
         <v>344</v>
-      </c>
-      <c r="N62" t="s" s="2">
-        <v>345</v>
       </c>
       <c r="O62" t="s" s="2">
         <v>42</v>
@@ -8160,14 +8156,14 @@
         <v>42</v>
       </c>
       <c r="W62" t="s" s="2">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="X62" t="s" s="2">
+        <v>345</v>
+      </c>
+      <c r="Y62" t="s" s="2">
         <v>346</v>
       </c>
-      <c r="Y62" t="s" s="2">
-        <v>347</v>
-      </c>
       <c r="Z62" t="s" s="2">
         <v>42</v>
       </c>
@@ -8184,7 +8180,7 @@
         <v>42</v>
       </c>
       <c r="AE62" t="s" s="2">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="AF62" t="s" s="2">
         <v>40</v>
@@ -8199,18 +8195,18 @@
         <v>42</v>
       </c>
       <c r="AJ62" t="s" s="2">
+        <v>347</v>
+      </c>
+      <c r="AK62" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AL62" t="s" s="2">
         <v>348</v>
-      </c>
-      <c r="AK62" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AL62" t="s" s="2">
-        <v>349</v>
       </c>
     </row>
     <row r="63" hidden="true">
       <c r="A63" t="s" s="2">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B63" s="2"/>
       <c r="C63" t="s" s="2">
@@ -8233,13 +8229,13 @@
         <v>42</v>
       </c>
       <c r="J63" t="s" s="2">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="K63" t="s" s="2">
+        <v>350</v>
+      </c>
+      <c r="L63" t="s" s="2">
         <v>351</v>
-      </c>
-      <c r="L63" t="s" s="2">
-        <v>352</v>
       </c>
       <c r="M63" s="2"/>
       <c r="N63" s="2"/>
@@ -8266,14 +8262,14 @@
         <v>42</v>
       </c>
       <c r="W63" t="s" s="2">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="X63" t="s" s="2">
+        <v>352</v>
+      </c>
+      <c r="Y63" t="s" s="2">
         <v>353</v>
       </c>
-      <c r="Y63" t="s" s="2">
-        <v>354</v>
-      </c>
       <c r="Z63" t="s" s="2">
         <v>42</v>
       </c>
@@ -8290,7 +8286,7 @@
         <v>42</v>
       </c>
       <c r="AE63" t="s" s="2">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="AF63" t="s" s="2">
         <v>40</v>
@@ -8305,18 +8301,18 @@
         <v>42</v>
       </c>
       <c r="AJ63" t="s" s="2">
+        <v>354</v>
+      </c>
+      <c r="AK63" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AL63" t="s" s="2">
         <v>355</v>
-      </c>
-      <c r="AK63" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AL63" t="s" s="2">
-        <v>356</v>
       </c>
     </row>
     <row r="64" hidden="true">
       <c r="A64" t="s" s="2">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B64" s="2"/>
       <c r="C64" t="s" s="2">
@@ -8339,13 +8335,13 @@
         <v>42</v>
       </c>
       <c r="J64" t="s" s="2">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="K64" t="s" s="2">
+        <v>357</v>
+      </c>
+      <c r="L64" t="s" s="2">
         <v>358</v>
-      </c>
-      <c r="L64" t="s" s="2">
-        <v>359</v>
       </c>
       <c r="M64" s="2"/>
       <c r="N64" s="2"/>
@@ -8372,14 +8368,14 @@
         <v>42</v>
       </c>
       <c r="W64" t="s" s="2">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="X64" t="s" s="2">
+        <v>359</v>
+      </c>
+      <c r="Y64" t="s" s="2">
         <v>360</v>
       </c>
-      <c r="Y64" t="s" s="2">
-        <v>361</v>
-      </c>
       <c r="Z64" t="s" s="2">
         <v>42</v>
       </c>
@@ -8396,7 +8392,7 @@
         <v>42</v>
       </c>
       <c r="AE64" t="s" s="2">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="AF64" t="s" s="2">
         <v>40</v>
@@ -8411,18 +8407,18 @@
         <v>42</v>
       </c>
       <c r="AJ64" t="s" s="2">
+        <v>361</v>
+      </c>
+      <c r="AK64" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AL64" t="s" s="2">
         <v>362</v>
-      </c>
-      <c r="AK64" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AL64" t="s" s="2">
-        <v>363</v>
       </c>
     </row>
     <row r="65" hidden="true">
       <c r="A65" t="s" s="2">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B65" s="2"/>
       <c r="C65" t="s" s="2">
@@ -8445,13 +8441,13 @@
         <v>42</v>
       </c>
       <c r="J65" t="s" s="2">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="K65" t="s" s="2">
+        <v>364</v>
+      </c>
+      <c r="L65" t="s" s="2">
         <v>365</v>
-      </c>
-      <c r="L65" t="s" s="2">
-        <v>366</v>
       </c>
       <c r="M65" s="2"/>
       <c r="N65" s="2"/>
@@ -8502,7 +8498,7 @@
         <v>42</v>
       </c>
       <c r="AE65" t="s" s="2">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="AF65" t="s" s="2">
         <v>40</v>
@@ -8517,18 +8513,18 @@
         <v>42</v>
       </c>
       <c r="AJ65" t="s" s="2">
+        <v>366</v>
+      </c>
+      <c r="AK65" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AL65" t="s" s="2">
         <v>367</v>
-      </c>
-      <c r="AK65" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AL65" t="s" s="2">
-        <v>368</v>
       </c>
     </row>
     <row r="66" hidden="true">
       <c r="A66" t="s" s="2">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B66" s="2"/>
       <c r="C66" t="s" s="2">
@@ -8551,13 +8547,13 @@
         <v>42</v>
       </c>
       <c r="J66" t="s" s="2">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="K66" t="s" s="2">
+        <v>369</v>
+      </c>
+      <c r="L66" t="s" s="2">
         <v>370</v>
-      </c>
-      <c r="L66" t="s" s="2">
-        <v>371</v>
       </c>
       <c r="M66" s="2"/>
       <c r="N66" s="2"/>
@@ -8584,14 +8580,14 @@
         <v>42</v>
       </c>
       <c r="W66" t="s" s="2">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="X66" t="s" s="2">
+        <v>371</v>
+      </c>
+      <c r="Y66" t="s" s="2">
         <v>372</v>
       </c>
-      <c r="Y66" t="s" s="2">
-        <v>373</v>
-      </c>
       <c r="Z66" t="s" s="2">
         <v>42</v>
       </c>
@@ -8608,7 +8604,7 @@
         <v>42</v>
       </c>
       <c r="AE66" t="s" s="2">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="AF66" t="s" s="2">
         <v>40</v>
@@ -8623,18 +8619,18 @@
         <v>42</v>
       </c>
       <c r="AJ66" t="s" s="2">
+        <v>373</v>
+      </c>
+      <c r="AK66" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AL66" t="s" s="2">
         <v>374</v>
-      </c>
-      <c r="AK66" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AL66" t="s" s="2">
-        <v>375</v>
       </c>
     </row>
     <row r="67" hidden="true">
       <c r="A67" t="s" s="2">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B67" s="2"/>
       <c r="C67" t="s" s="2">
@@ -8657,13 +8653,13 @@
         <v>42</v>
       </c>
       <c r="J67" t="s" s="2">
+        <v>141</v>
+      </c>
+      <c r="K67" t="s" s="2">
         <v>142</v>
       </c>
-      <c r="K67" t="s" s="2">
+      <c r="L67" t="s" s="2">
         <v>143</v>
-      </c>
-      <c r="L67" t="s" s="2">
-        <v>144</v>
       </c>
       <c r="M67" s="2"/>
       <c r="N67" s="2"/>
@@ -8714,7 +8710,7 @@
         <v>42</v>
       </c>
       <c r="AE67" t="s" s="2">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="AF67" t="s" s="2">
         <v>40</v>
@@ -8729,7 +8725,7 @@
         <v>42</v>
       </c>
       <c r="AJ67" t="s" s="2">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AK67" t="s" s="2">
         <v>42</v>
@@ -8740,11 +8736,11 @@
     </row>
     <row r="68" hidden="true">
       <c r="A68" t="s" s="2">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B68" s="2"/>
       <c r="C68" t="s" s="2">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D68" s="2"/>
       <c r="E68" t="s" s="2">
@@ -8766,13 +8762,13 @@
         <v>94</v>
       </c>
       <c r="K68" t="s" s="2">
+        <v>146</v>
+      </c>
+      <c r="L68" t="s" s="2">
         <v>147</v>
       </c>
-      <c r="L68" t="s" s="2">
-        <v>148</v>
-      </c>
       <c r="M68" t="s" s="2">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="N68" s="2"/>
       <c r="O68" t="s" s="2">
@@ -8813,7 +8809,7 @@
         <v>97</v>
       </c>
       <c r="AB68" t="s" s="2">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="AC68" t="s" s="2">
         <v>42</v>
@@ -8822,7 +8818,7 @@
         <v>98</v>
       </c>
       <c r="AE68" t="s" s="2">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="AF68" t="s" s="2">
         <v>40</v>
@@ -8837,7 +8833,7 @@
         <v>42</v>
       </c>
       <c r="AJ68" t="s" s="2">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AK68" t="s" s="2">
         <v>42</v>
@@ -8848,7 +8844,7 @@
     </row>
     <row r="69" hidden="true">
       <c r="A69" t="s" s="2">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B69" s="2"/>
       <c r="C69" t="s" s="2">
@@ -8871,19 +8867,19 @@
         <v>50</v>
       </c>
       <c r="J69" t="s" s="2">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K69" t="s" s="2">
+        <v>379</v>
+      </c>
+      <c r="L69" t="s" s="2">
         <v>380</v>
       </c>
-      <c r="L69" t="s" s="2">
+      <c r="M69" t="s" s="2">
         <v>381</v>
       </c>
-      <c r="M69" t="s" s="2">
+      <c r="N69" t="s" s="2">
         <v>382</v>
-      </c>
-      <c r="N69" t="s" s="2">
-        <v>383</v>
       </c>
       <c r="O69" t="s" s="2">
         <v>42</v>
@@ -8920,7 +8916,7 @@
         <v>42</v>
       </c>
       <c r="AA69" t="s" s="2">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="AB69" s="2"/>
       <c r="AC69" t="s" s="2">
@@ -8930,7 +8926,7 @@
         <v>98</v>
       </c>
       <c r="AE69" t="s" s="2">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="AF69" t="s" s="2">
         <v>40</v>
@@ -8945,21 +8941,21 @@
         <v>42</v>
       </c>
       <c r="AJ69" t="s" s="2">
+        <v>385</v>
+      </c>
+      <c r="AK69" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AL69" t="s" s="2">
         <v>386</v>
-      </c>
-      <c r="AK69" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AL69" t="s" s="2">
-        <v>387</v>
       </c>
     </row>
     <row r="70" hidden="true">
       <c r="A70" t="s" s="2">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B70" t="s" s="2">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="C70" t="s" s="2">
         <v>42</v>
@@ -8981,19 +8977,19 @@
         <v>50</v>
       </c>
       <c r="J70" t="s" s="2">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K70" t="s" s="2">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="L70" t="s" s="2">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="M70" t="s" s="2">
+        <v>381</v>
+      </c>
+      <c r="N70" t="s" s="2">
         <v>382</v>
-      </c>
-      <c r="N70" t="s" s="2">
-        <v>383</v>
       </c>
       <c r="O70" t="s" s="2">
         <v>42</v>
@@ -9018,11 +9014,11 @@
         <v>42</v>
       </c>
       <c r="W70" t="s" s="2">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="X70" s="2"/>
       <c r="Y70" t="s" s="2">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="Z70" t="s" s="2">
         <v>42</v>
@@ -9040,7 +9036,7 @@
         <v>42</v>
       </c>
       <c r="AE70" t="s" s="2">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="AF70" t="s" s="2">
         <v>40</v>
@@ -9055,18 +9051,18 @@
         <v>42</v>
       </c>
       <c r="AJ70" t="s" s="2">
+        <v>385</v>
+      </c>
+      <c r="AK70" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AL70" t="s" s="2">
         <v>386</v>
-      </c>
-      <c r="AK70" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AL70" t="s" s="2">
-        <v>387</v>
       </c>
     </row>
     <row r="71" hidden="true">
       <c r="A71" t="s" s="2">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B71" s="2"/>
       <c r="C71" t="s" s="2">
@@ -9089,19 +9085,19 @@
         <v>50</v>
       </c>
       <c r="J71" t="s" s="2">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="K71" t="s" s="2">
+        <v>391</v>
+      </c>
+      <c r="L71" t="s" s="2">
         <v>392</v>
       </c>
-      <c r="L71" t="s" s="2">
+      <c r="M71" t="s" s="2">
         <v>393</v>
       </c>
-      <c r="M71" t="s" s="2">
+      <c r="N71" t="s" s="2">
         <v>394</v>
-      </c>
-      <c r="N71" t="s" s="2">
-        <v>395</v>
       </c>
       <c r="O71" t="s" s="2">
         <v>42</v>
@@ -9150,7 +9146,7 @@
         <v>42</v>
       </c>
       <c r="AE71" t="s" s="2">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="AF71" t="s" s="2">
         <v>40</v>
@@ -9165,18 +9161,18 @@
         <v>42</v>
       </c>
       <c r="AJ71" t="s" s="2">
+        <v>396</v>
+      </c>
+      <c r="AK71" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AL71" t="s" s="2">
         <v>397</v>
-      </c>
-      <c r="AK71" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AL71" t="s" s="2">
-        <v>398</v>
       </c>
     </row>
     <row r="72" hidden="true">
       <c r="A72" t="s" s="2">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="B72" s="2"/>
       <c r="C72" t="s" s="2">
@@ -9199,16 +9195,16 @@
         <v>42</v>
       </c>
       <c r="J72" t="s" s="2">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K72" t="s" s="2">
+        <v>399</v>
+      </c>
+      <c r="L72" t="s" s="2">
         <v>400</v>
       </c>
-      <c r="L72" t="s" s="2">
+      <c r="M72" t="s" s="2">
         <v>401</v>
-      </c>
-      <c r="M72" t="s" s="2">
-        <v>402</v>
       </c>
       <c r="N72" s="2"/>
       <c r="O72" t="s" s="2">
@@ -9258,7 +9254,7 @@
         <v>42</v>
       </c>
       <c r="AE72" t="s" s="2">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="AF72" t="s" s="2">
         <v>40</v>
@@ -9270,10 +9266,10 @@
         <v>42</v>
       </c>
       <c r="AI72" t="s" s="2">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="AJ72" t="s" s="2">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="AK72" t="s" s="2">
         <v>42</v>
@@ -9284,7 +9280,7 @@
     </row>
     <row r="73" hidden="true">
       <c r="A73" t="s" s="2">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B73" s="2"/>
       <c r="C73" t="s" s="2">
@@ -9307,13 +9303,13 @@
         <v>42</v>
       </c>
       <c r="J73" t="s" s="2">
+        <v>141</v>
+      </c>
+      <c r="K73" t="s" s="2">
         <v>142</v>
       </c>
-      <c r="K73" t="s" s="2">
+      <c r="L73" t="s" s="2">
         <v>143</v>
-      </c>
-      <c r="L73" t="s" s="2">
-        <v>144</v>
       </c>
       <c r="M73" s="2"/>
       <c r="N73" s="2"/>
@@ -9364,7 +9360,7 @@
         <v>42</v>
       </c>
       <c r="AE73" t="s" s="2">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="AF73" t="s" s="2">
         <v>40</v>
@@ -9379,7 +9375,7 @@
         <v>42</v>
       </c>
       <c r="AJ73" t="s" s="2">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AK73" t="s" s="2">
         <v>42</v>
@@ -9390,11 +9386,11 @@
     </row>
     <row r="74" hidden="true">
       <c r="A74" t="s" s="2">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B74" s="2"/>
       <c r="C74" t="s" s="2">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D74" s="2"/>
       <c r="E74" t="s" s="2">
@@ -9416,13 +9412,13 @@
         <v>94</v>
       </c>
       <c r="K74" t="s" s="2">
+        <v>146</v>
+      </c>
+      <c r="L74" t="s" s="2">
         <v>147</v>
       </c>
-      <c r="L74" t="s" s="2">
-        <v>148</v>
-      </c>
       <c r="M74" t="s" s="2">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="N74" s="2"/>
       <c r="O74" t="s" s="2">
@@ -9472,7 +9468,7 @@
         <v>42</v>
       </c>
       <c r="AE74" t="s" s="2">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="AF74" t="s" s="2">
         <v>40</v>
@@ -9487,7 +9483,7 @@
         <v>42</v>
       </c>
       <c r="AJ74" t="s" s="2">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AK74" t="s" s="2">
         <v>42</v>
@@ -9498,11 +9494,11 @@
     </row>
     <row r="75" hidden="true">
       <c r="A75" t="s" s="2">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B75" s="2"/>
       <c r="C75" t="s" s="2">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D75" s="2"/>
       <c r="E75" t="s" s="2">
@@ -9524,13 +9520,13 @@
         <v>94</v>
       </c>
       <c r="K75" t="s" s="2">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="L75" t="s" s="2">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="M75" t="s" s="2">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="N75" s="2"/>
       <c r="O75" t="s" s="2">
@@ -9580,7 +9576,7 @@
         <v>42</v>
       </c>
       <c r="AE75" t="s" s="2">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AF75" t="s" s="2">
         <v>40</v>
@@ -9606,7 +9602,7 @@
     </row>
     <row r="76" hidden="true">
       <c r="A76" t="s" s="2">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B76" s="2"/>
       <c r="C76" t="s" s="2">
@@ -9629,13 +9625,13 @@
         <v>42</v>
       </c>
       <c r="J76" t="s" s="2">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="K76" t="s" s="2">
+        <v>407</v>
+      </c>
+      <c r="L76" t="s" s="2">
         <v>408</v>
-      </c>
-      <c r="L76" t="s" s="2">
-        <v>409</v>
       </c>
       <c r="M76" s="2"/>
       <c r="N76" s="2"/>
@@ -9686,7 +9682,7 @@
         <v>42</v>
       </c>
       <c r="AE76" t="s" s="2">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="AF76" t="s" s="2">
         <v>49</v>
@@ -9701,18 +9697,18 @@
         <v>42</v>
       </c>
       <c r="AJ76" t="s" s="2">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="AK76" t="s" s="2">
+        <v>409</v>
+      </c>
+      <c r="AL76" t="s" s="2">
         <v>410</v>
-      </c>
-      <c r="AL76" t="s" s="2">
-        <v>411</v>
       </c>
     </row>
     <row r="77" hidden="true">
       <c r="A77" t="s" s="2">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B77" s="2"/>
       <c r="C77" t="s" s="2">
@@ -9738,13 +9734,13 @@
         <v>68</v>
       </c>
       <c r="K77" t="s" s="2">
+        <v>412</v>
+      </c>
+      <c r="L77" t="s" s="2">
         <v>413</v>
       </c>
-      <c r="L77" t="s" s="2">
+      <c r="M77" t="s" s="2">
         <v>414</v>
-      </c>
-      <c r="M77" t="s" s="2">
-        <v>415</v>
       </c>
       <c r="N77" s="2"/>
       <c r="O77" t="s" s="2">
@@ -9770,14 +9766,14 @@
         <v>42</v>
       </c>
       <c r="W77" t="s" s="2">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="X77" t="s" s="2">
+        <v>415</v>
+      </c>
+      <c r="Y77" t="s" s="2">
         <v>416</v>
       </c>
-      <c r="Y77" t="s" s="2">
-        <v>417</v>
-      </c>
       <c r="Z77" t="s" s="2">
         <v>42</v>
       </c>
@@ -9794,7 +9790,7 @@
         <v>42</v>
       </c>
       <c r="AE77" t="s" s="2">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="AF77" t="s" s="2">
         <v>40</v>
@@ -9809,7 +9805,7 @@
         <v>42</v>
       </c>
       <c r="AJ77" t="s" s="2">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="AK77" t="s" s="2">
         <v>42</v>
@@ -9820,7 +9816,7 @@
     </row>
     <row r="78" hidden="true">
       <c r="A78" t="s" s="2">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B78" s="2"/>
       <c r="C78" t="s" s="2">
@@ -9843,13 +9839,13 @@
         <v>42</v>
       </c>
       <c r="J78" t="s" s="2">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="K78" t="s" s="2">
+        <v>419</v>
+      </c>
+      <c r="L78" t="s" s="2">
         <v>420</v>
-      </c>
-      <c r="L78" t="s" s="2">
-        <v>421</v>
       </c>
       <c r="M78" s="2"/>
       <c r="N78" s="2"/>
@@ -9900,7 +9896,7 @@
         <v>42</v>
       </c>
       <c r="AE78" t="s" s="2">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="AF78" t="s" s="2">
         <v>40</v>
@@ -9915,7 +9911,7 @@
         <v>42</v>
       </c>
       <c r="AJ78" t="s" s="2">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="AK78" t="s" s="2">
         <v>42</v>
@@ -9926,7 +9922,7 @@
     </row>
     <row r="79" hidden="true">
       <c r="A79" t="s" s="2">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B79" s="2"/>
       <c r="C79" t="s" s="2">
@@ -9949,13 +9945,13 @@
         <v>42</v>
       </c>
       <c r="J79" t="s" s="2">
+        <v>422</v>
+      </c>
+      <c r="K79" t="s" s="2">
         <v>423</v>
       </c>
-      <c r="K79" t="s" s="2">
+      <c r="L79" t="s" s="2">
         <v>424</v>
-      </c>
-      <c r="L79" t="s" s="2">
-        <v>425</v>
       </c>
       <c r="M79" s="2"/>
       <c r="N79" s="2"/>
@@ -10006,7 +10002,7 @@
         <v>42</v>
       </c>
       <c r="AE79" t="s" s="2">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="AF79" t="s" s="2">
         <v>40</v>
@@ -10021,18 +10017,18 @@
         <v>42</v>
       </c>
       <c r="AJ79" t="s" s="2">
+        <v>425</v>
+      </c>
+      <c r="AK79" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AL79" t="s" s="2">
         <v>426</v>
-      </c>
-      <c r="AK79" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AL79" t="s" s="2">
-        <v>427</v>
       </c>
     </row>
     <row r="80" hidden="true">
       <c r="A80" t="s" s="2">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="B80" s="2"/>
       <c r="C80" t="s" s="2">
@@ -10055,16 +10051,16 @@
         <v>42</v>
       </c>
       <c r="J80" t="s" s="2">
+        <v>428</v>
+      </c>
+      <c r="K80" t="s" s="2">
         <v>429</v>
       </c>
-      <c r="K80" t="s" s="2">
+      <c r="L80" t="s" s="2">
         <v>430</v>
       </c>
-      <c r="L80" t="s" s="2">
+      <c r="M80" t="s" s="2">
         <v>431</v>
-      </c>
-      <c r="M80" t="s" s="2">
-        <v>432</v>
       </c>
       <c r="N80" s="2"/>
       <c r="O80" t="s" s="2">
@@ -10114,7 +10110,7 @@
         <v>42</v>
       </c>
       <c r="AE80" t="s" s="2">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="AF80" t="s" s="2">
         <v>40</v>
@@ -10129,7 +10125,7 @@
         <v>42</v>
       </c>
       <c r="AJ80" t="s" s="2">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="AK80" t="s" s="2">
         <v>42</v>

</xml_diff>

<commit_message>
Updated invariants of an Encounter for an Event  and generated the output for ES CIFMM-2704
</commit_message>
<xml_diff>
--- a/output/EventSummary/encounter-es-1.xlsx
+++ b/output/EventSummary/encounter-es-1.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2685" uniqueCount="433">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2685" uniqueCount="432">
   <si>
     <t>Path</t>
   </si>
@@ -154,7 +154,7 @@
   </si>
   <si>
     <t>dom-2:If the resource is contained in another resource, it SHALL NOT contain nested Resources {contained.contained.empty()}
-dom-1:If the resource is contained in another resource, it SHALL NOT contain any narrative {contained.text.empty()}dom-4:If a resource is contained in another resource, it SHALL NOT have a meta.versionId or a meta.lastUpdated {contained.meta.versionId.empty() and contained.meta.lastUpdated.empty()}dom-3:If the resource is contained in another resource, it SHALL be referred to from elsewhere in the resource {contained.where(('#'+id in %resource.descendants().reference).not()).empty()}</t>
+dom-1:If the resource is contained in another resource, it SHALL NOT contain any narrative {contained.text.empty()}dom-4:If a resource is contained in another resource, it SHALL NOT have a meta.versionId or a meta.lastUpdated {contained.meta.versionId.empty() and contained.meta.lastUpdated.empty()}dom-3:If the resource is contained in another resource, it SHALL be referred to from elsewhere in the resource {contained.where(('#'+id in %resource.descendants().reference).not()).empty()}inv-dh-enc-01:The subject shall at least have a reference or an identifier with at least a system and a value {subject.reference.exists() or subject.identifier.where(system.count() + value.count() &gt;1).exists()}</t>
   </si>
   <si>
     <t>Encounter[@moodCode='EVN']</t>
@@ -646,10 +646,6 @@
   </si>
   <si>
     <t>While the encounter is always about the patient, the patient may not actually be known in all contexts of use, and there may be a group of patients that could be anonymous (such as in a group therapy for Alcoholics Anonymous - where the recording of the encounter could be used for billing on the number of people/staff and not important to the context of the specific patients) or alternately in veterinary care a herd of sheep receiving treatment (where the animals are not individually tracked).</t>
-  </si>
-  <si>
-    <t xml:space="preserve">inv-dh-enc-01:The subject shall at least have a reference or an identifier {reference.exists() or identifier.exists()}
-</t>
   </si>
   <si>
     <t>.participation[typeCode=SBJ]/role[classCode=PAT]</t>
@@ -4769,21 +4765,21 @@
         <v>42</v>
       </c>
       <c r="AI30" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AJ30" t="s" s="2">
         <v>200</v>
       </c>
-      <c r="AJ30" t="s" s="2">
+      <c r="AK30" t="s" s="2">
         <v>201</v>
       </c>
-      <c r="AK30" t="s" s="2">
+      <c r="AL30" t="s" s="2">
         <v>202</v>
-      </c>
-      <c r="AL30" t="s" s="2">
-        <v>203</v>
       </c>
     </row>
     <row r="31" hidden="true">
       <c r="A31" t="s" s="2">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" t="s" s="2">
@@ -4806,13 +4802,13 @@
         <v>50</v>
       </c>
       <c r="J31" t="s" s="2">
+        <v>204</v>
+      </c>
+      <c r="K31" t="s" s="2">
         <v>205</v>
       </c>
-      <c r="K31" t="s" s="2">
+      <c r="L31" t="s" s="2">
         <v>206</v>
-      </c>
-      <c r="L31" t="s" s="2">
-        <v>207</v>
       </c>
       <c r="M31" s="2"/>
       <c r="N31" s="2"/>
@@ -4863,7 +4859,7 @@
         <v>42</v>
       </c>
       <c r="AE31" t="s" s="2">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="AF31" t="s" s="2">
         <v>40</v>
@@ -4881,15 +4877,15 @@
         <v>139</v>
       </c>
       <c r="AK31" t="s" s="2">
+        <v>207</v>
+      </c>
+      <c r="AL31" t="s" s="2">
         <v>208</v>
-      </c>
-      <c r="AL31" t="s" s="2">
-        <v>209</v>
       </c>
     </row>
     <row r="32" hidden="true">
       <c r="A32" t="s" s="2">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B32" s="2"/>
       <c r="C32" t="s" s="2">
@@ -4912,13 +4908,13 @@
         <v>42</v>
       </c>
       <c r="J32" t="s" s="2">
+        <v>210</v>
+      </c>
+      <c r="K32" t="s" s="2">
         <v>211</v>
       </c>
-      <c r="K32" t="s" s="2">
+      <c r="L32" t="s" s="2">
         <v>212</v>
-      </c>
-      <c r="L32" t="s" s="2">
-        <v>213</v>
       </c>
       <c r="M32" s="2"/>
       <c r="N32" s="2"/>
@@ -4969,7 +4965,7 @@
         <v>42</v>
       </c>
       <c r="AE32" t="s" s="2">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="AF32" t="s" s="2">
         <v>40</v>
@@ -4984,7 +4980,7 @@
         <v>42</v>
       </c>
       <c r="AJ32" t="s" s="2">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="AK32" t="s" s="2">
         <v>42</v>
@@ -4995,7 +4991,7 @@
     </row>
     <row r="33" hidden="true">
       <c r="A33" t="s" s="2">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" t="s" s="2">
@@ -5021,10 +5017,10 @@
         <v>134</v>
       </c>
       <c r="K33" t="s" s="2">
+        <v>215</v>
+      </c>
+      <c r="L33" t="s" s="2">
         <v>216</v>
-      </c>
-      <c r="L33" t="s" s="2">
-        <v>217</v>
       </c>
       <c r="M33" s="2"/>
       <c r="N33" s="2"/>
@@ -5075,7 +5071,7 @@
         <v>42</v>
       </c>
       <c r="AE33" t="s" s="2">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="AF33" t="s" s="2">
         <v>40</v>
@@ -5090,18 +5086,18 @@
         <v>138</v>
       </c>
       <c r="AJ33" t="s" s="2">
+        <v>217</v>
+      </c>
+      <c r="AK33" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AL33" t="s" s="2">
         <v>218</v>
-      </c>
-      <c r="AK33" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AL33" t="s" s="2">
-        <v>219</v>
       </c>
     </row>
     <row r="34" hidden="true">
       <c r="A34" t="s" s="2">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B34" s="2"/>
       <c r="C34" t="s" s="2">
@@ -5207,7 +5203,7 @@
     </row>
     <row r="35" hidden="true">
       <c r="A35" t="s" s="2">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" t="s" s="2">
@@ -5315,7 +5311,7 @@
     </row>
     <row r="36" hidden="true">
       <c r="A36" t="s" s="2">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B36" s="2"/>
       <c r="C36" t="s" s="2">
@@ -5423,7 +5419,7 @@
     </row>
     <row r="37" hidden="true">
       <c r="A37" t="s" s="2">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" t="s" s="2">
@@ -5449,13 +5445,13 @@
         <v>178</v>
       </c>
       <c r="K37" t="s" s="2">
+        <v>223</v>
+      </c>
+      <c r="L37" t="s" s="2">
         <v>224</v>
       </c>
-      <c r="L37" t="s" s="2">
+      <c r="M37" t="s" s="2">
         <v>225</v>
-      </c>
-      <c r="M37" t="s" s="2">
-        <v>226</v>
       </c>
       <c r="N37" s="2"/>
       <c r="O37" t="s" s="2">
@@ -5484,10 +5480,10 @@
         <v>72</v>
       </c>
       <c r="X37" t="s" s="2">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="Y37" t="s" s="2">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="Z37" t="s" s="2">
         <v>42</v>
@@ -5505,7 +5501,7 @@
         <v>42</v>
       </c>
       <c r="AE37" t="s" s="2">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="AF37" t="s" s="2">
         <v>40</v>
@@ -5520,18 +5516,18 @@
         <v>42</v>
       </c>
       <c r="AJ37" t="s" s="2">
+        <v>227</v>
+      </c>
+      <c r="AK37" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AL37" t="s" s="2">
         <v>228</v>
-      </c>
-      <c r="AK37" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AL37" t="s" s="2">
-        <v>229</v>
       </c>
     </row>
     <row r="38" hidden="true">
       <c r="A38" t="s" s="2">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B38" s="2"/>
       <c r="C38" t="s" s="2">
@@ -5557,10 +5553,10 @@
         <v>155</v>
       </c>
       <c r="K38" t="s" s="2">
+        <v>230</v>
+      </c>
+      <c r="L38" t="s" s="2">
         <v>231</v>
-      </c>
-      <c r="L38" t="s" s="2">
-        <v>232</v>
       </c>
       <c r="M38" s="2"/>
       <c r="N38" s="2"/>
@@ -5611,7 +5607,7 @@
         <v>42</v>
       </c>
       <c r="AE38" t="s" s="2">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="AF38" t="s" s="2">
         <v>40</v>
@@ -5626,18 +5622,18 @@
         <v>42</v>
       </c>
       <c r="AJ38" t="s" s="2">
+        <v>232</v>
+      </c>
+      <c r="AK38" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AL38" t="s" s="2">
         <v>233</v>
-      </c>
-      <c r="AK38" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AL38" t="s" s="2">
-        <v>234</v>
       </c>
     </row>
     <row r="39" hidden="true">
       <c r="A39" t="s" s="2">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B39" s="2"/>
       <c r="C39" t="s" s="2">
@@ -5660,13 +5656,13 @@
         <v>50</v>
       </c>
       <c r="J39" t="s" s="2">
+        <v>235</v>
+      </c>
+      <c r="K39" t="s" s="2">
         <v>236</v>
       </c>
-      <c r="K39" t="s" s="2">
+      <c r="L39" t="s" s="2">
         <v>237</v>
-      </c>
-      <c r="L39" t="s" s="2">
-        <v>238</v>
       </c>
       <c r="M39" s="2"/>
       <c r="N39" s="2"/>
@@ -5717,7 +5713,7 @@
         <v>42</v>
       </c>
       <c r="AE39" t="s" s="2">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="AF39" t="s" s="2">
         <v>40</v>
@@ -5732,18 +5728,18 @@
         <v>42</v>
       </c>
       <c r="AJ39" t="s" s="2">
+        <v>238</v>
+      </c>
+      <c r="AK39" t="s" s="2">
         <v>239</v>
       </c>
-      <c r="AK39" t="s" s="2">
+      <c r="AL39" t="s" s="2">
         <v>240</v>
-      </c>
-      <c r="AL39" t="s" s="2">
-        <v>241</v>
       </c>
     </row>
     <row r="40" hidden="true">
       <c r="A40" t="s" s="2">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B40" s="2"/>
       <c r="C40" t="s" s="2">
@@ -5766,13 +5762,13 @@
         <v>50</v>
       </c>
       <c r="J40" t="s" s="2">
+        <v>242</v>
+      </c>
+      <c r="K40" t="s" s="2">
         <v>243</v>
       </c>
-      <c r="K40" t="s" s="2">
+      <c r="L40" t="s" s="2">
         <v>244</v>
-      </c>
-      <c r="L40" t="s" s="2">
-        <v>245</v>
       </c>
       <c r="M40" s="2"/>
       <c r="N40" s="2"/>
@@ -5823,7 +5819,7 @@
         <v>42</v>
       </c>
       <c r="AE40" t="s" s="2">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="AF40" t="s" s="2">
         <v>40</v>
@@ -5838,18 +5834,18 @@
         <v>42</v>
       </c>
       <c r="AJ40" t="s" s="2">
+        <v>245</v>
+      </c>
+      <c r="AK40" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AL40" t="s" s="2">
         <v>246</v>
-      </c>
-      <c r="AK40" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AL40" t="s" s="2">
-        <v>247</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s" s="2">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" t="s" s="2">
@@ -5875,13 +5871,13 @@
         <v>155</v>
       </c>
       <c r="K41" t="s" s="2">
+        <v>248</v>
+      </c>
+      <c r="L41" t="s" s="2">
         <v>249</v>
       </c>
-      <c r="L41" t="s" s="2">
+      <c r="M41" t="s" s="2">
         <v>250</v>
-      </c>
-      <c r="M41" t="s" s="2">
-        <v>251</v>
       </c>
       <c r="N41" s="2"/>
       <c r="O41" t="s" s="2">
@@ -5931,7 +5927,7 @@
         <v>42</v>
       </c>
       <c r="AE41" t="s" s="2">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="AF41" t="s" s="2">
         <v>40</v>
@@ -5946,18 +5942,18 @@
         <v>42</v>
       </c>
       <c r="AJ41" t="s" s="2">
+        <v>251</v>
+      </c>
+      <c r="AK41" t="s" s="2">
         <v>252</v>
       </c>
-      <c r="AK41" t="s" s="2">
+      <c r="AL41" t="s" s="2">
         <v>253</v>
-      </c>
-      <c r="AL41" t="s" s="2">
-        <v>254</v>
       </c>
     </row>
     <row r="42" hidden="true">
       <c r="A42" t="s" s="2">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B42" s="2"/>
       <c r="C42" t="s" s="2">
@@ -5980,16 +5976,16 @@
         <v>42</v>
       </c>
       <c r="J42" t="s" s="2">
+        <v>255</v>
+      </c>
+      <c r="K42" t="s" s="2">
         <v>256</v>
       </c>
-      <c r="K42" t="s" s="2">
+      <c r="L42" t="s" s="2">
         <v>257</v>
       </c>
-      <c r="L42" t="s" s="2">
+      <c r="M42" t="s" s="2">
         <v>258</v>
-      </c>
-      <c r="M42" t="s" s="2">
-        <v>259</v>
       </c>
       <c r="N42" s="2"/>
       <c r="O42" t="s" s="2">
@@ -6039,7 +6035,7 @@
         <v>42</v>
       </c>
       <c r="AE42" t="s" s="2">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="AF42" t="s" s="2">
         <v>40</v>
@@ -6054,22 +6050,22 @@
         <v>42</v>
       </c>
       <c r="AJ42" t="s" s="2">
+        <v>259</v>
+      </c>
+      <c r="AK42" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AL42" t="s" s="2">
         <v>260</v>
-      </c>
-      <c r="AK42" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AL42" t="s" s="2">
-        <v>261</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s" s="2">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" t="s" s="2">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D43" s="2"/>
       <c r="E43" t="s" s="2">
@@ -6091,13 +6087,13 @@
         <v>178</v>
       </c>
       <c r="K43" t="s" s="2">
+        <v>263</v>
+      </c>
+      <c r="L43" t="s" s="2">
         <v>264</v>
       </c>
-      <c r="L43" t="s" s="2">
+      <c r="M43" t="s" s="2">
         <v>265</v>
-      </c>
-      <c r="M43" t="s" s="2">
-        <v>266</v>
       </c>
       <c r="N43" s="2"/>
       <c r="O43" t="s" s="2">
@@ -6126,11 +6122,11 @@
         <v>182</v>
       </c>
       <c r="X43" t="s" s="2">
+        <v>266</v>
+      </c>
+      <c r="Y43" t="s" s="2">
         <v>267</v>
       </c>
-      <c r="Y43" t="s" s="2">
-        <v>268</v>
-      </c>
       <c r="Z43" t="s" s="2">
         <v>42</v>
       </c>
@@ -6147,7 +6143,7 @@
         <v>42</v>
       </c>
       <c r="AE43" t="s" s="2">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="AF43" t="s" s="2">
         <v>40</v>
@@ -6162,18 +6158,18 @@
         <v>42</v>
       </c>
       <c r="AJ43" t="s" s="2">
+        <v>268</v>
+      </c>
+      <c r="AK43" t="s" s="2">
         <v>269</v>
       </c>
-      <c r="AK43" t="s" s="2">
+      <c r="AL43" t="s" s="2">
         <v>270</v>
-      </c>
-      <c r="AL43" t="s" s="2">
-        <v>271</v>
       </c>
     </row>
     <row r="44" hidden="true">
       <c r="A44" t="s" s="2">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B44" s="2"/>
       <c r="C44" t="s" s="2">
@@ -6199,10 +6195,10 @@
         <v>134</v>
       </c>
       <c r="K44" t="s" s="2">
+        <v>272</v>
+      </c>
+      <c r="L44" t="s" s="2">
         <v>273</v>
-      </c>
-      <c r="L44" t="s" s="2">
-        <v>274</v>
       </c>
       <c r="M44" s="2"/>
       <c r="N44" s="2"/>
@@ -6253,7 +6249,7 @@
         <v>42</v>
       </c>
       <c r="AE44" t="s" s="2">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="AF44" t="s" s="2">
         <v>40</v>
@@ -6268,7 +6264,7 @@
         <v>138</v>
       </c>
       <c r="AJ44" t="s" s="2">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="AK44" t="s" s="2">
         <v>42</v>
@@ -6279,7 +6275,7 @@
     </row>
     <row r="45" hidden="true">
       <c r="A45" t="s" s="2">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B45" s="2"/>
       <c r="C45" t="s" s="2">
@@ -6385,7 +6381,7 @@
     </row>
     <row r="46" hidden="true">
       <c r="A46" t="s" s="2">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B46" s="2"/>
       <c r="C46" t="s" s="2">
@@ -6493,7 +6489,7 @@
     </row>
     <row r="47" hidden="true">
       <c r="A47" t="s" s="2">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B47" s="2"/>
       <c r="C47" t="s" s="2">
@@ -6601,11 +6597,11 @@
     </row>
     <row r="48" hidden="true">
       <c r="A48" t="s" s="2">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B48" s="2"/>
       <c r="C48" t="s" s="2">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D48" s="2"/>
       <c r="E48" t="s" s="2">
@@ -6624,16 +6620,16 @@
         <v>42</v>
       </c>
       <c r="J48" t="s" s="2">
+        <v>280</v>
+      </c>
+      <c r="K48" t="s" s="2">
         <v>281</v>
       </c>
-      <c r="K48" t="s" s="2">
+      <c r="L48" t="s" s="2">
         <v>282</v>
       </c>
-      <c r="L48" t="s" s="2">
-        <v>283</v>
-      </c>
       <c r="M48" t="s" s="2">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="N48" s="2"/>
       <c r="O48" t="s" s="2">
@@ -6683,7 +6679,7 @@
         <v>42</v>
       </c>
       <c r="AE48" t="s" s="2">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="AF48" t="s" s="2">
         <v>49</v>
@@ -6698,18 +6694,18 @@
         <v>42</v>
       </c>
       <c r="AJ48" t="s" s="2">
+        <v>283</v>
+      </c>
+      <c r="AK48" t="s" s="2">
+        <v>269</v>
+      </c>
+      <c r="AL48" t="s" s="2">
         <v>284</v>
-      </c>
-      <c r="AK48" t="s" s="2">
-        <v>270</v>
-      </c>
-      <c r="AL48" t="s" s="2">
-        <v>285</v>
       </c>
     </row>
     <row r="49" hidden="true">
       <c r="A49" t="s" s="2">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B49" s="2"/>
       <c r="C49" t="s" s="2">
@@ -6735,10 +6731,10 @@
         <v>178</v>
       </c>
       <c r="K49" t="s" s="2">
+        <v>286</v>
+      </c>
+      <c r="L49" t="s" s="2">
         <v>287</v>
-      </c>
-      <c r="L49" t="s" s="2">
-        <v>288</v>
       </c>
       <c r="M49" s="2"/>
       <c r="N49" s="2"/>
@@ -6768,11 +6764,11 @@
         <v>182</v>
       </c>
       <c r="X49" t="s" s="2">
+        <v>288</v>
+      </c>
+      <c r="Y49" t="s" s="2">
         <v>289</v>
       </c>
-      <c r="Y49" t="s" s="2">
-        <v>290</v>
-      </c>
       <c r="Z49" t="s" s="2">
         <v>42</v>
       </c>
@@ -6789,7 +6785,7 @@
         <v>42</v>
       </c>
       <c r="AE49" t="s" s="2">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="AF49" t="s" s="2">
         <v>40</v>
@@ -6815,7 +6811,7 @@
     </row>
     <row r="50" hidden="true">
       <c r="A50" t="s" s="2">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B50" s="2"/>
       <c r="C50" t="s" s="2">
@@ -6838,13 +6834,13 @@
         <v>42</v>
       </c>
       <c r="J50" t="s" s="2">
+        <v>291</v>
+      </c>
+      <c r="K50" t="s" s="2">
         <v>292</v>
       </c>
-      <c r="K50" t="s" s="2">
+      <c r="L50" t="s" s="2">
         <v>293</v>
-      </c>
-      <c r="L50" t="s" s="2">
-        <v>294</v>
       </c>
       <c r="M50" s="2"/>
       <c r="N50" s="2"/>
@@ -6895,7 +6891,7 @@
         <v>42</v>
       </c>
       <c r="AE50" t="s" s="2">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="AF50" t="s" s="2">
         <v>40</v>
@@ -6910,7 +6906,7 @@
         <v>42</v>
       </c>
       <c r="AJ50" t="s" s="2">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="AK50" t="s" s="2">
         <v>42</v>
@@ -6921,7 +6917,7 @@
     </row>
     <row r="51" hidden="true">
       <c r="A51" t="s" s="2">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B51" s="2"/>
       <c r="C51" t="s" s="2">
@@ -6944,16 +6940,16 @@
         <v>42</v>
       </c>
       <c r="J51" t="s" s="2">
+        <v>296</v>
+      </c>
+      <c r="K51" t="s" s="2">
         <v>297</v>
       </c>
-      <c r="K51" t="s" s="2">
+      <c r="L51" t="s" s="2">
         <v>298</v>
       </c>
-      <c r="L51" t="s" s="2">
+      <c r="M51" t="s" s="2">
         <v>299</v>
-      </c>
-      <c r="M51" t="s" s="2">
-        <v>300</v>
       </c>
       <c r="N51" s="2"/>
       <c r="O51" t="s" s="2">
@@ -7003,7 +6999,7 @@
         <v>42</v>
       </c>
       <c r="AE51" t="s" s="2">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="AF51" t="s" s="2">
         <v>40</v>
@@ -7018,7 +7014,7 @@
         <v>42</v>
       </c>
       <c r="AJ51" t="s" s="2">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="AK51" t="s" s="2">
         <v>42</v>
@@ -7029,7 +7025,7 @@
     </row>
     <row r="52" hidden="true">
       <c r="A52" t="s" s="2">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B52" s="2"/>
       <c r="C52" t="s" s="2">
@@ -7055,13 +7051,13 @@
         <v>134</v>
       </c>
       <c r="K52" t="s" s="2">
+        <v>302</v>
+      </c>
+      <c r="L52" t="s" s="2">
         <v>303</v>
       </c>
-      <c r="L52" t="s" s="2">
+      <c r="M52" t="s" s="2">
         <v>304</v>
-      </c>
-      <c r="M52" t="s" s="2">
-        <v>305</v>
       </c>
       <c r="N52" s="2"/>
       <c r="O52" t="s" s="2">
@@ -7111,7 +7107,7 @@
         <v>42</v>
       </c>
       <c r="AE52" t="s" s="2">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="AF52" t="s" s="2">
         <v>40</v>
@@ -7126,7 +7122,7 @@
         <v>138</v>
       </c>
       <c r="AJ52" t="s" s="2">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="AK52" t="s" s="2">
         <v>42</v>
@@ -7137,7 +7133,7 @@
     </row>
     <row r="53" hidden="true">
       <c r="A53" t="s" s="2">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B53" s="2"/>
       <c r="C53" t="s" s="2">
@@ -7243,7 +7239,7 @@
     </row>
     <row r="54" hidden="true">
       <c r="A54" t="s" s="2">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B54" s="2"/>
       <c r="C54" t="s" s="2">
@@ -7347,10 +7343,10 @@
     </row>
     <row r="55" hidden="true">
       <c r="A55" t="s" s="2">
+        <v>307</v>
+      </c>
+      <c r="B55" t="s" s="2">
         <v>308</v>
-      </c>
-      <c r="B55" t="s" s="2">
-        <v>309</v>
       </c>
       <c r="C55" t="s" s="2">
         <v>42</v>
@@ -7372,13 +7368,13 @@
         <v>42</v>
       </c>
       <c r="J55" t="s" s="2">
+        <v>309</v>
+      </c>
+      <c r="K55" t="s" s="2">
         <v>310</v>
       </c>
-      <c r="K55" t="s" s="2">
+      <c r="L55" t="s" s="2">
         <v>311</v>
-      </c>
-      <c r="L55" t="s" s="2">
-        <v>312</v>
       </c>
       <c r="M55" s="2"/>
       <c r="N55" s="2"/>
@@ -7455,10 +7451,10 @@
     </row>
     <row r="56" hidden="true">
       <c r="A56" t="s" s="2">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B56" t="s" s="2">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C56" t="s" s="2">
         <v>42</v>
@@ -7480,13 +7476,13 @@
         <v>42</v>
       </c>
       <c r="J56" t="s" s="2">
+        <v>313</v>
+      </c>
+      <c r="K56" t="s" s="2">
         <v>314</v>
       </c>
-      <c r="K56" t="s" s="2">
+      <c r="L56" t="s" s="2">
         <v>315</v>
-      </c>
-      <c r="L56" t="s" s="2">
-        <v>316</v>
       </c>
       <c r="M56" s="2"/>
       <c r="N56" s="2"/>
@@ -7563,7 +7559,7 @@
     </row>
     <row r="57" hidden="true">
       <c r="A57" t="s" s="2">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B57" s="2"/>
       <c r="C57" t="s" s="2">
@@ -7671,7 +7667,7 @@
     </row>
     <row r="58" hidden="true">
       <c r="A58" t="s" s="2">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B58" s="2"/>
       <c r="C58" t="s" s="2">
@@ -7697,10 +7693,10 @@
         <v>117</v>
       </c>
       <c r="K58" t="s" s="2">
+        <v>318</v>
+      </c>
+      <c r="L58" t="s" s="2">
         <v>319</v>
-      </c>
-      <c r="L58" t="s" s="2">
-        <v>320</v>
       </c>
       <c r="M58" s="2"/>
       <c r="N58" s="2"/>
@@ -7751,7 +7747,7 @@
         <v>42</v>
       </c>
       <c r="AE58" t="s" s="2">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="AF58" t="s" s="2">
         <v>40</v>
@@ -7772,12 +7768,12 @@
         <v>42</v>
       </c>
       <c r="AL58" t="s" s="2">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="59" hidden="true">
       <c r="A59" t="s" s="2">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B59" s="2"/>
       <c r="C59" t="s" s="2">
@@ -7800,13 +7796,13 @@
         <v>42</v>
       </c>
       <c r="J59" t="s" s="2">
+        <v>322</v>
+      </c>
+      <c r="K59" t="s" s="2">
         <v>323</v>
       </c>
-      <c r="K59" t="s" s="2">
+      <c r="L59" t="s" s="2">
         <v>324</v>
-      </c>
-      <c r="L59" t="s" s="2">
-        <v>325</v>
       </c>
       <c r="M59" s="2"/>
       <c r="N59" s="2"/>
@@ -7857,7 +7853,7 @@
         <v>42</v>
       </c>
       <c r="AE59" t="s" s="2">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="AF59" t="s" s="2">
         <v>40</v>
@@ -7872,7 +7868,7 @@
         <v>42</v>
       </c>
       <c r="AJ59" t="s" s="2">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="AK59" t="s" s="2">
         <v>42</v>
@@ -7883,7 +7879,7 @@
     </row>
     <row r="60" hidden="true">
       <c r="A60" t="s" s="2">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B60" s="2"/>
       <c r="C60" t="s" s="2">
@@ -7909,10 +7905,10 @@
         <v>178</v>
       </c>
       <c r="K60" t="s" s="2">
+        <v>327</v>
+      </c>
+      <c r="L60" t="s" s="2">
         <v>328</v>
-      </c>
-      <c r="L60" t="s" s="2">
-        <v>329</v>
       </c>
       <c r="M60" s="2"/>
       <c r="N60" s="2"/>
@@ -7942,11 +7938,11 @@
         <v>182</v>
       </c>
       <c r="X60" t="s" s="2">
+        <v>329</v>
+      </c>
+      <c r="Y60" t="s" s="2">
         <v>330</v>
       </c>
-      <c r="Y60" t="s" s="2">
-        <v>331</v>
-      </c>
       <c r="Z60" t="s" s="2">
         <v>42</v>
       </c>
@@ -7963,7 +7959,7 @@
         <v>42</v>
       </c>
       <c r="AE60" t="s" s="2">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="AF60" t="s" s="2">
         <v>40</v>
@@ -7978,18 +7974,18 @@
         <v>42</v>
       </c>
       <c r="AJ60" t="s" s="2">
+        <v>331</v>
+      </c>
+      <c r="AK60" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AL60" t="s" s="2">
         <v>332</v>
-      </c>
-      <c r="AK60" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AL60" t="s" s="2">
-        <v>333</v>
       </c>
     </row>
     <row r="61" hidden="true">
       <c r="A61" t="s" s="2">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B61" s="2"/>
       <c r="C61" t="s" s="2">
@@ -8015,10 +8011,10 @@
         <v>178</v>
       </c>
       <c r="K61" t="s" s="2">
+        <v>334</v>
+      </c>
+      <c r="L61" t="s" s="2">
         <v>335</v>
-      </c>
-      <c r="L61" t="s" s="2">
-        <v>336</v>
       </c>
       <c r="M61" s="2"/>
       <c r="N61" s="2"/>
@@ -8048,11 +8044,11 @@
         <v>189</v>
       </c>
       <c r="X61" t="s" s="2">
+        <v>336</v>
+      </c>
+      <c r="Y61" t="s" s="2">
         <v>337</v>
       </c>
-      <c r="Y61" t="s" s="2">
-        <v>338</v>
-      </c>
       <c r="Z61" t="s" s="2">
         <v>42</v>
       </c>
@@ -8069,7 +8065,7 @@
         <v>42</v>
       </c>
       <c r="AE61" t="s" s="2">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="AF61" t="s" s="2">
         <v>40</v>
@@ -8090,12 +8086,12 @@
         <v>42</v>
       </c>
       <c r="AL61" t="s" s="2">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="62" hidden="true">
       <c r="A62" t="s" s="2">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B62" s="2"/>
       <c r="C62" t="s" s="2">
@@ -8121,16 +8117,16 @@
         <v>178</v>
       </c>
       <c r="K62" t="s" s="2">
+        <v>340</v>
+      </c>
+      <c r="L62" t="s" s="2">
         <v>341</v>
       </c>
-      <c r="L62" t="s" s="2">
+      <c r="M62" t="s" s="2">
         <v>342</v>
       </c>
-      <c r="M62" t="s" s="2">
+      <c r="N62" t="s" s="2">
         <v>343</v>
-      </c>
-      <c r="N62" t="s" s="2">
-        <v>344</v>
       </c>
       <c r="O62" t="s" s="2">
         <v>42</v>
@@ -8158,11 +8154,11 @@
         <v>189</v>
       </c>
       <c r="X62" t="s" s="2">
+        <v>344</v>
+      </c>
+      <c r="Y62" t="s" s="2">
         <v>345</v>
       </c>
-      <c r="Y62" t="s" s="2">
-        <v>346</v>
-      </c>
       <c r="Z62" t="s" s="2">
         <v>42</v>
       </c>
@@ -8179,7 +8175,7 @@
         <v>42</v>
       </c>
       <c r="AE62" t="s" s="2">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="AF62" t="s" s="2">
         <v>40</v>
@@ -8194,18 +8190,18 @@
         <v>42</v>
       </c>
       <c r="AJ62" t="s" s="2">
+        <v>346</v>
+      </c>
+      <c r="AK62" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AL62" t="s" s="2">
         <v>347</v>
-      </c>
-      <c r="AK62" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AL62" t="s" s="2">
-        <v>348</v>
       </c>
     </row>
     <row r="63" hidden="true">
       <c r="A63" t="s" s="2">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B63" s="2"/>
       <c r="C63" t="s" s="2">
@@ -8231,10 +8227,10 @@
         <v>178</v>
       </c>
       <c r="K63" t="s" s="2">
+        <v>349</v>
+      </c>
+      <c r="L63" t="s" s="2">
         <v>350</v>
-      </c>
-      <c r="L63" t="s" s="2">
-        <v>351</v>
       </c>
       <c r="M63" s="2"/>
       <c r="N63" s="2"/>
@@ -8264,11 +8260,11 @@
         <v>182</v>
       </c>
       <c r="X63" t="s" s="2">
+        <v>351</v>
+      </c>
+      <c r="Y63" t="s" s="2">
         <v>352</v>
       </c>
-      <c r="Y63" t="s" s="2">
-        <v>353</v>
-      </c>
       <c r="Z63" t="s" s="2">
         <v>42</v>
       </c>
@@ -8285,7 +8281,7 @@
         <v>42</v>
       </c>
       <c r="AE63" t="s" s="2">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="AF63" t="s" s="2">
         <v>40</v>
@@ -8300,18 +8296,18 @@
         <v>42</v>
       </c>
       <c r="AJ63" t="s" s="2">
+        <v>353</v>
+      </c>
+      <c r="AK63" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AL63" t="s" s="2">
         <v>354</v>
-      </c>
-      <c r="AK63" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AL63" t="s" s="2">
-        <v>355</v>
       </c>
     </row>
     <row r="64" hidden="true">
       <c r="A64" t="s" s="2">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B64" s="2"/>
       <c r="C64" t="s" s="2">
@@ -8337,10 +8333,10 @@
         <v>178</v>
       </c>
       <c r="K64" t="s" s="2">
+        <v>356</v>
+      </c>
+      <c r="L64" t="s" s="2">
         <v>357</v>
-      </c>
-      <c r="L64" t="s" s="2">
-        <v>358</v>
       </c>
       <c r="M64" s="2"/>
       <c r="N64" s="2"/>
@@ -8370,11 +8366,11 @@
         <v>182</v>
       </c>
       <c r="X64" t="s" s="2">
+        <v>358</v>
+      </c>
+      <c r="Y64" t="s" s="2">
         <v>359</v>
       </c>
-      <c r="Y64" t="s" s="2">
-        <v>360</v>
-      </c>
       <c r="Z64" t="s" s="2">
         <v>42</v>
       </c>
@@ -8391,7 +8387,7 @@
         <v>42</v>
       </c>
       <c r="AE64" t="s" s="2">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="AF64" t="s" s="2">
         <v>40</v>
@@ -8406,18 +8402,18 @@
         <v>42</v>
       </c>
       <c r="AJ64" t="s" s="2">
+        <v>360</v>
+      </c>
+      <c r="AK64" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AL64" t="s" s="2">
         <v>361</v>
-      </c>
-      <c r="AK64" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AL64" t="s" s="2">
-        <v>362</v>
       </c>
     </row>
     <row r="65" hidden="true">
       <c r="A65" t="s" s="2">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B65" s="2"/>
       <c r="C65" t="s" s="2">
@@ -8440,13 +8436,13 @@
         <v>42</v>
       </c>
       <c r="J65" t="s" s="2">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="K65" t="s" s="2">
+        <v>363</v>
+      </c>
+      <c r="L65" t="s" s="2">
         <v>364</v>
-      </c>
-      <c r="L65" t="s" s="2">
-        <v>365</v>
       </c>
       <c r="M65" s="2"/>
       <c r="N65" s="2"/>
@@ -8497,7 +8493,7 @@
         <v>42</v>
       </c>
       <c r="AE65" t="s" s="2">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="AF65" t="s" s="2">
         <v>40</v>
@@ -8512,18 +8508,18 @@
         <v>42</v>
       </c>
       <c r="AJ65" t="s" s="2">
+        <v>365</v>
+      </c>
+      <c r="AK65" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AL65" t="s" s="2">
         <v>366</v>
-      </c>
-      <c r="AK65" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AL65" t="s" s="2">
-        <v>367</v>
       </c>
     </row>
     <row r="66" hidden="true">
       <c r="A66" t="s" s="2">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B66" s="2"/>
       <c r="C66" t="s" s="2">
@@ -8549,10 +8545,10 @@
         <v>178</v>
       </c>
       <c r="K66" t="s" s="2">
+        <v>368</v>
+      </c>
+      <c r="L66" t="s" s="2">
         <v>369</v>
-      </c>
-      <c r="L66" t="s" s="2">
-        <v>370</v>
       </c>
       <c r="M66" s="2"/>
       <c r="N66" s="2"/>
@@ -8582,11 +8578,11 @@
         <v>189</v>
       </c>
       <c r="X66" t="s" s="2">
+        <v>370</v>
+      </c>
+      <c r="Y66" t="s" s="2">
         <v>371</v>
       </c>
-      <c r="Y66" t="s" s="2">
-        <v>372</v>
-      </c>
       <c r="Z66" t="s" s="2">
         <v>42</v>
       </c>
@@ -8603,7 +8599,7 @@
         <v>42</v>
       </c>
       <c r="AE66" t="s" s="2">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="AF66" t="s" s="2">
         <v>40</v>
@@ -8618,18 +8614,18 @@
         <v>42</v>
       </c>
       <c r="AJ66" t="s" s="2">
+        <v>372</v>
+      </c>
+      <c r="AK66" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AL66" t="s" s="2">
         <v>373</v>
-      </c>
-      <c r="AK66" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AL66" t="s" s="2">
-        <v>374</v>
       </c>
     </row>
     <row r="67" hidden="true">
       <c r="A67" t="s" s="2">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B67" s="2"/>
       <c r="C67" t="s" s="2">
@@ -8735,7 +8731,7 @@
     </row>
     <row r="68" hidden="true">
       <c r="A68" t="s" s="2">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B68" s="2"/>
       <c r="C68" t="s" s="2">
@@ -8808,7 +8804,7 @@
         <v>97</v>
       </c>
       <c r="AB68" t="s" s="2">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="AC68" t="s" s="2">
         <v>42</v>
@@ -8843,7 +8839,7 @@
     </row>
     <row r="69" hidden="true">
       <c r="A69" t="s" s="2">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B69" s="2"/>
       <c r="C69" t="s" s="2">
@@ -8869,16 +8865,16 @@
         <v>159</v>
       </c>
       <c r="K69" t="s" s="2">
+        <v>378</v>
+      </c>
+      <c r="L69" t="s" s="2">
         <v>379</v>
       </c>
-      <c r="L69" t="s" s="2">
+      <c r="M69" t="s" s="2">
         <v>380</v>
       </c>
-      <c r="M69" t="s" s="2">
+      <c r="N69" t="s" s="2">
         <v>381</v>
-      </c>
-      <c r="N69" t="s" s="2">
-        <v>382</v>
       </c>
       <c r="O69" t="s" s="2">
         <v>42</v>
@@ -8915,7 +8911,7 @@
         <v>42</v>
       </c>
       <c r="AA69" t="s" s="2">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="AB69" s="2"/>
       <c r="AC69" t="s" s="2">
@@ -8925,7 +8921,7 @@
         <v>98</v>
       </c>
       <c r="AE69" t="s" s="2">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="AF69" t="s" s="2">
         <v>40</v>
@@ -8940,21 +8936,21 @@
         <v>42</v>
       </c>
       <c r="AJ69" t="s" s="2">
+        <v>384</v>
+      </c>
+      <c r="AK69" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AL69" t="s" s="2">
         <v>385</v>
-      </c>
-      <c r="AK69" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AL69" t="s" s="2">
-        <v>386</v>
       </c>
     </row>
     <row r="70" hidden="true">
       <c r="A70" t="s" s="2">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B70" t="s" s="2">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="C70" t="s" s="2">
         <v>42</v>
@@ -8979,16 +8975,16 @@
         <v>159</v>
       </c>
       <c r="K70" t="s" s="2">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="L70" t="s" s="2">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="M70" t="s" s="2">
+        <v>380</v>
+      </c>
+      <c r="N70" t="s" s="2">
         <v>381</v>
-      </c>
-      <c r="N70" t="s" s="2">
-        <v>382</v>
       </c>
       <c r="O70" t="s" s="2">
         <v>42</v>
@@ -9017,7 +9013,7 @@
       </c>
       <c r="X70" s="2"/>
       <c r="Y70" t="s" s="2">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="Z70" t="s" s="2">
         <v>42</v>
@@ -9035,7 +9031,7 @@
         <v>42</v>
       </c>
       <c r="AE70" t="s" s="2">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="AF70" t="s" s="2">
         <v>40</v>
@@ -9050,18 +9046,18 @@
         <v>42</v>
       </c>
       <c r="AJ70" t="s" s="2">
+        <v>384</v>
+      </c>
+      <c r="AK70" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AL70" t="s" s="2">
         <v>385</v>
-      </c>
-      <c r="AK70" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AL70" t="s" s="2">
-        <v>386</v>
       </c>
     </row>
     <row r="71" hidden="true">
       <c r="A71" t="s" s="2">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B71" s="2"/>
       <c r="C71" t="s" s="2">
@@ -9087,16 +9083,16 @@
         <v>141</v>
       </c>
       <c r="K71" t="s" s="2">
+        <v>390</v>
+      </c>
+      <c r="L71" t="s" s="2">
         <v>391</v>
       </c>
-      <c r="L71" t="s" s="2">
+      <c r="M71" t="s" s="2">
         <v>392</v>
       </c>
-      <c r="M71" t="s" s="2">
+      <c r="N71" t="s" s="2">
         <v>393</v>
-      </c>
-      <c r="N71" t="s" s="2">
-        <v>394</v>
       </c>
       <c r="O71" t="s" s="2">
         <v>42</v>
@@ -9145,7 +9141,7 @@
         <v>42</v>
       </c>
       <c r="AE71" t="s" s="2">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="AF71" t="s" s="2">
         <v>40</v>
@@ -9160,18 +9156,18 @@
         <v>42</v>
       </c>
       <c r="AJ71" t="s" s="2">
+        <v>395</v>
+      </c>
+      <c r="AK71" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AL71" t="s" s="2">
         <v>396</v>
-      </c>
-      <c r="AK71" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AL71" t="s" s="2">
-        <v>397</v>
       </c>
     </row>
     <row r="72" hidden="true">
       <c r="A72" t="s" s="2">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="B72" s="2"/>
       <c r="C72" t="s" s="2">
@@ -9197,13 +9193,13 @@
         <v>134</v>
       </c>
       <c r="K72" t="s" s="2">
+        <v>398</v>
+      </c>
+      <c r="L72" t="s" s="2">
         <v>399</v>
       </c>
-      <c r="L72" t="s" s="2">
+      <c r="M72" t="s" s="2">
         <v>400</v>
-      </c>
-      <c r="M72" t="s" s="2">
-        <v>401</v>
       </c>
       <c r="N72" s="2"/>
       <c r="O72" t="s" s="2">
@@ -9253,7 +9249,7 @@
         <v>42</v>
       </c>
       <c r="AE72" t="s" s="2">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="AF72" t="s" s="2">
         <v>40</v>
@@ -9268,7 +9264,7 @@
         <v>138</v>
       </c>
       <c r="AJ72" t="s" s="2">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="AK72" t="s" s="2">
         <v>42</v>
@@ -9279,7 +9275,7 @@
     </row>
     <row r="73" hidden="true">
       <c r="A73" t="s" s="2">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="B73" s="2"/>
       <c r="C73" t="s" s="2">
@@ -9385,7 +9381,7 @@
     </row>
     <row r="74" hidden="true">
       <c r="A74" t="s" s="2">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B74" s="2"/>
       <c r="C74" t="s" s="2">
@@ -9493,7 +9489,7 @@
     </row>
     <row r="75" hidden="true">
       <c r="A75" t="s" s="2">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B75" s="2"/>
       <c r="C75" t="s" s="2">
@@ -9601,7 +9597,7 @@
     </row>
     <row r="76" hidden="true">
       <c r="A76" t="s" s="2">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B76" s="2"/>
       <c r="C76" t="s" s="2">
@@ -9624,13 +9620,13 @@
         <v>42</v>
       </c>
       <c r="J76" t="s" s="2">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="K76" t="s" s="2">
+        <v>406</v>
+      </c>
+      <c r="L76" t="s" s="2">
         <v>407</v>
-      </c>
-      <c r="L76" t="s" s="2">
-        <v>408</v>
       </c>
       <c r="M76" s="2"/>
       <c r="N76" s="2"/>
@@ -9681,7 +9677,7 @@
         <v>42</v>
       </c>
       <c r="AE76" t="s" s="2">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="AF76" t="s" s="2">
         <v>49</v>
@@ -9696,18 +9692,18 @@
         <v>42</v>
       </c>
       <c r="AJ76" t="s" s="2">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="AK76" t="s" s="2">
+        <v>408</v>
+      </c>
+      <c r="AL76" t="s" s="2">
         <v>409</v>
-      </c>
-      <c r="AL76" t="s" s="2">
-        <v>410</v>
       </c>
     </row>
     <row r="77" hidden="true">
       <c r="A77" t="s" s="2">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B77" s="2"/>
       <c r="C77" t="s" s="2">
@@ -9733,13 +9729,13 @@
         <v>68</v>
       </c>
       <c r="K77" t="s" s="2">
+        <v>411</v>
+      </c>
+      <c r="L77" t="s" s="2">
         <v>412</v>
       </c>
-      <c r="L77" t="s" s="2">
+      <c r="M77" t="s" s="2">
         <v>413</v>
-      </c>
-      <c r="M77" t="s" s="2">
-        <v>414</v>
       </c>
       <c r="N77" s="2"/>
       <c r="O77" t="s" s="2">
@@ -9768,11 +9764,11 @@
         <v>127</v>
       </c>
       <c r="X77" t="s" s="2">
+        <v>414</v>
+      </c>
+      <c r="Y77" t="s" s="2">
         <v>415</v>
       </c>
-      <c r="Y77" t="s" s="2">
-        <v>416</v>
-      </c>
       <c r="Z77" t="s" s="2">
         <v>42</v>
       </c>
@@ -9789,7 +9785,7 @@
         <v>42</v>
       </c>
       <c r="AE77" t="s" s="2">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="AF77" t="s" s="2">
         <v>40</v>
@@ -9804,7 +9800,7 @@
         <v>42</v>
       </c>
       <c r="AJ77" t="s" s="2">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="AK77" t="s" s="2">
         <v>42</v>
@@ -9815,7 +9811,7 @@
     </row>
     <row r="78" hidden="true">
       <c r="A78" t="s" s="2">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B78" s="2"/>
       <c r="C78" t="s" s="2">
@@ -9841,10 +9837,10 @@
         <v>155</v>
       </c>
       <c r="K78" t="s" s="2">
+        <v>418</v>
+      </c>
+      <c r="L78" t="s" s="2">
         <v>419</v>
-      </c>
-      <c r="L78" t="s" s="2">
-        <v>420</v>
       </c>
       <c r="M78" s="2"/>
       <c r="N78" s="2"/>
@@ -9895,7 +9891,7 @@
         <v>42</v>
       </c>
       <c r="AE78" t="s" s="2">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="AF78" t="s" s="2">
         <v>40</v>
@@ -9910,7 +9906,7 @@
         <v>42</v>
       </c>
       <c r="AJ78" t="s" s="2">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="AK78" t="s" s="2">
         <v>42</v>
@@ -9921,7 +9917,7 @@
     </row>
     <row r="79" hidden="true">
       <c r="A79" t="s" s="2">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="B79" s="2"/>
       <c r="C79" t="s" s="2">
@@ -9944,13 +9940,13 @@
         <v>42</v>
       </c>
       <c r="J79" t="s" s="2">
+        <v>421</v>
+      </c>
+      <c r="K79" t="s" s="2">
         <v>422</v>
       </c>
-      <c r="K79" t="s" s="2">
+      <c r="L79" t="s" s="2">
         <v>423</v>
-      </c>
-      <c r="L79" t="s" s="2">
-        <v>424</v>
       </c>
       <c r="M79" s="2"/>
       <c r="N79" s="2"/>
@@ -10001,7 +9997,7 @@
         <v>42</v>
       </c>
       <c r="AE79" t="s" s="2">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="AF79" t="s" s="2">
         <v>40</v>
@@ -10016,18 +10012,18 @@
         <v>42</v>
       </c>
       <c r="AJ79" t="s" s="2">
+        <v>424</v>
+      </c>
+      <c r="AK79" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AL79" t="s" s="2">
         <v>425</v>
-      </c>
-      <c r="AK79" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AL79" t="s" s="2">
-        <v>426</v>
       </c>
     </row>
     <row r="80" hidden="true">
       <c r="A80" t="s" s="2">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B80" s="2"/>
       <c r="C80" t="s" s="2">
@@ -10050,16 +10046,16 @@
         <v>42</v>
       </c>
       <c r="J80" t="s" s="2">
+        <v>427</v>
+      </c>
+      <c r="K80" t="s" s="2">
         <v>428</v>
       </c>
-      <c r="K80" t="s" s="2">
+      <c r="L80" t="s" s="2">
         <v>429</v>
       </c>
-      <c r="L80" t="s" s="2">
+      <c r="M80" t="s" s="2">
         <v>430</v>
-      </c>
-      <c r="M80" t="s" s="2">
-        <v>431</v>
       </c>
       <c r="N80" s="2"/>
       <c r="O80" t="s" s="2">
@@ -10109,7 +10105,7 @@
         <v>42</v>
       </c>
       <c r="AE80" t="s" s="2">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="AF80" t="s" s="2">
         <v>40</v>
@@ -10124,7 +10120,7 @@
         <v>42</v>
       </c>
       <c r="AJ80" t="s" s="2">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="AK80" t="s" s="2">
         <v>42</v>

</xml_diff>

<commit_message>
ES IG - regeneration of outputs following multiple updates
- Event Summary composition profile - bug in AuthorRole extension invariant
- Incorrect use of fixedCodeableConcept in various profiles
- Event Summary - improve implementation guidance esp around lists and medicine changes
- Update Event Summary composition to add a rule that the encounter shall have encounter description
- Event Summary composition profile - missing constraints on elements with a Reference
- Event Summary Composition - invariant FHIRPaths are absolute and need to be relative

CIFMM-2682
</commit_message>
<xml_diff>
--- a/output/EventSummary/encounter-es-1.xlsx
+++ b/output/EventSummary/encounter-es-1.xlsx
@@ -595,7 +595,7 @@
     <t>preferred</t>
   </si>
   <si>
-    <t>https://healthterminologies.gov.au/fhir/ValueSet/medicines-review-type-2</t>
+    <t>https://healthterminologies.gov.au/fhir/ValueSet/encounter-type-1</t>
   </si>
   <si>
     <t>.code</t>
@@ -1470,7 +1470,7 @@
     <col min="22" max="22" width="17.078125" customWidth="true" bestFit="true"/>
     <col min="23" max="23" width="16.30859375" customWidth="true" bestFit="true"/>
     <col min="24" max="24" width="72.9921875" customWidth="true" bestFit="true"/>
-    <col min="25" max="25" width="68.2734375" customWidth="true" bestFit="true"/>
+    <col min="25" max="25" width="63.2421875" customWidth="true" bestFit="true"/>
     <col min="26" max="26" width="5.69140625" customWidth="true" bestFit="true"/>
     <col min="27" max="27" width="19.73046875" customWidth="true" bestFit="true"/>
     <col min="28" max="28" width="17.8203125" customWidth="true" bestFit="true"/>

</xml_diff>